<commit_message>
Sign In and Logout
Change input logout, return userlogid when sign in account
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -66,26 +66,6 @@
   </si>
   <si>
     <t>user_id</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "message": {
-            "code": 200,
-            "message": "Logout successfully."
-        }
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "message": {
-            "code": 404,
-            "message": "The user does not already exists."
-        }
-    }
-}</t>
   </si>
   <si>
     <t>upload_avatar</t>
@@ -3842,53 +3822,85 @@
   </si>
   <si>
     <t>{
-    "autoUserId": "1",
-    "userId": "1-1",
-    "tsUserId": "1-1",
-    "tsUserEmail": "hphu90@gmail.com",
-    "tsUserPw": "abcde",
-    "tsFirstName": "Phan",
-    "tsLastName": "Phu",
-    "maxInvites": "100",
-    "userCreatedInitialDatetime": "",
-    "userPoints": "0",
-    "twitterUsrUrl": "",
-    "userDisabledFlag": "",
-    "userActivationKey": "",
-    "userGender": "",
-    "userCityId": "",
-    "userState": "",
-    "isOnline": "n",
-    "userCountry": "",
-    "about": "",
-    "currentStatus": "e",
-    "userFbId": ""
+    "user_log_id": "20130701171352-1-1-10",
+    "user": {
+        "autoUserId": "1",
+        "userId": "1-1",
+        "tsUserId": "1-1",
+        "tsUserEmail": "hphu90@gmail.com",
+        "tsUserPw": "abcde",
+        "tsFirstName": "Phan",
+        "tsLastName": "Phu",
+        "maxInvites": "100",
+        "userCreatedInitialDatetime": "",
+        "userPoints": "0",
+        "twitterUsrUrl": "",
+        "userDisabledFlag": "",
+        "userActivationKey": "",
+        "userGender": "",
+        "userCityId": "",
+        "userState": "",
+        "isOnline": "y",
+        "userCountry": "",
+        "about": "",
+        "currentStatus": "e",
+        "userFbId": ""
+    },
+    "user_profile_obj": null,
+    "user_data": null,
+    "city": null,
+    "fb_user_data": null,
+    "list_user_data": null,
+    "list_user": null,
+    "list_user_follow_data": null,
+    "list_fb_user_data": null,
+    "list_cities": null
 }</t>
   </si>
   <si>
     <t>{
-    "autoUserId": "9",
-    "userId": "1-9",
-    "tsUserId": "1-9",
-    "tsUserEmail": "tanhuu94_dn@gmail.com",
-    "tsUserPw": "",
-    "tsFirstName": "Phan",
-    "tsLastName": "Huu",
-    "maxInvites": "100",
-    "userCreatedInitialDatetime": "2013-06-28 09:51:16.0",
-    "userPoints": "0",
-    "twitterUsrUrl": "",
-    "userDisabledFlag": "",
-    "userActivationKey": "",
-    "userGender": "male",
-    "userCityId": "1",
-    "userState": "VN",
-    "isOnline": "y",
-    "userCountry": "VN",
-    "about": "",
-    "currentStatus": "e",
-    "userFbId": "1143242"
+    "successMsg": "Logout success!"
 }</t>
+  </si>
+  <si>
+    <t>{
+    "user_log_id": "20130701180200-1-9-14",
+    "user": {
+        "autoUserId": "9",
+        "userId": "1-9",
+        "tsUserId": "1-9",
+        "tsUserEmail": "tanhuu94_dn@gmail.com",
+        "tsUserPw": "",
+        "tsFirstName": "Phan",
+        "tsLastName": "Huu",
+        "maxInvites": "100",
+        "userCreatedInitialDatetime": "2013-06-28 09:51:16.0",
+        "userPoints": "0",
+        "twitterUsrUrl": "",
+        "userDisabledFlag": "",
+        "userActivationKey": "",
+        "userGender": "male",
+        "userCityId": "1",
+        "userState": "VN",
+        "isOnline": "y",
+        "userCountry": "VN",
+        "about": "",
+        "currentStatus": "e",
+        "userFbId": "1143242"
+    },
+    "user_profile_obj": null,
+    "user_data": null,
+    "city": null,
+    "fb_user_data": null,
+    "list_user_data": null,
+    "list_user": null,
+    "list_user_follow_data": null,
+    "list_fb_user_data": null,
+    "list_cities": null
+}</t>
+  </si>
+  <si>
+    <t>userLogId</t>
   </si>
 </sst>
 </file>
@@ -4062,21 +4074,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4235,6 +4232,21 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4540,1717 +4552,1717 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1"/>
-    <col min="2" max="2" width="8" style="48" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="8" style="43" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="38" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="3"/>
     <col min="5" max="5" width="34" style="3" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="46.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="43.5703125" style="56" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" style="51" customWidth="1"/>
     <col min="9" max="9" width="17.140625" style="2"/>
     <col min="10" max="10" width="17.140625" style="4"/>
     <col min="11" max="11" width="30.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" style="28" customWidth="1"/>
-    <col min="13" max="13" width="56.42578125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="41.140625" style="28" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="23" customWidth="1"/>
+    <col min="13" max="13" width="56.42578125" style="23" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" style="23" customWidth="1"/>
     <col min="15" max="15" width="73.42578125" style="4" customWidth="1"/>
     <col min="16" max="16384" width="17.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:25" s="12" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:25" s="7" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="E2" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" s="12" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="25"/>
+      <c r="M3" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>214</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="L5" s="25"/>
+      <c r="M5" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="59"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-    </row>
-    <row r="3" spans="1:25" s="17" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="H6" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="27"/>
+      <c r="M6" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+    </row>
+    <row r="8" spans="1:25" s="8" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="59"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="27"/>
+      <c r="M8" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="59"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="59"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="27"/>
+      <c r="M10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="59"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="12" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="27"/>
+    </row>
+    <row r="17" spans="1:14" s="12" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="25"/>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="27"/>
+    </row>
+    <row r="19" spans="1:14" s="12" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="N19" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="8" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="59"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="N21" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="59"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="12" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="59"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="25"/>
+      <c r="M23" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L24" s="27"/>
+      <c r="M24" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N24" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="59"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L25" s="25"/>
+      <c r="M25" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="59"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L26" s="27"/>
+      <c r="M26" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="59"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="K27" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="L27" s="25"/>
+      <c r="M27" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="59"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H28" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="27"/>
+      <c r="M28" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="N28" s="26"/>
+    </row>
+    <row r="29" spans="1:14" s="16" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="15"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+    </row>
+    <row r="30" spans="1:14" s="12" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="49"/>
+      <c r="C30" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="N30" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="61"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N31" s="33"/>
+    </row>
+    <row r="32" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="61"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="20"/>
+      <c r="K32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="32"/>
+      <c r="M32" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="61"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N33" s="33"/>
+    </row>
+    <row r="34" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="61"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="N34" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="61"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" s="11"/>
+      <c r="H35" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35" s="33"/>
+    </row>
+    <row r="36" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="61"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="20"/>
+      <c r="H36" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="N36" s="32"/>
+    </row>
+    <row r="37" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="H37" s="53"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+    </row>
+    <row r="38" spans="1:15" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="18"/>
+      <c r="H38" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="N38" s="30"/>
+    </row>
+    <row r="39" spans="1:15" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="63"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="53" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="G39" s="11"/>
+      <c r="H39" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="33"/>
+      <c r="M39" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="63"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E40" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="N3" s="33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" s="13" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="C4" s="42" t="s">
+      <c r="F40" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="H40" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="20"/>
+      <c r="K40" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L40" s="32"/>
+      <c r="M40" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="N40" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="63"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="11"/>
+      <c r="H41" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="K41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="63"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="M42" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="63"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N43" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="63"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+    </row>
+    <row r="45" spans="1:15" s="8" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="37"/>
+      <c r="H45" s="57"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+    </row>
+    <row r="46" spans="1:15" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="49"/>
+      <c r="C46" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E46" s="18"/>
+      <c r="F46" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="18"/>
+      <c r="H46" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="N46" s="30"/>
+      <c r="O46" s="18"/>
+    </row>
+    <row r="47" spans="1:15" s="8" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="63"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="57" t="s">
-        <v>219</v>
-      </c>
-      <c r="I4" s="14" t="s">
+      <c r="E47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="L47" s="33"/>
+      <c r="M47" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="N47" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="O47" s="11"/>
+    </row>
+    <row r="48" spans="1:15" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="63"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="N48" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="63"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L49" s="33"/>
+      <c r="M49" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="N49" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="63"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50" s="20"/>
+      <c r="H50" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="20"/>
+      <c r="K50" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="L50" s="32"/>
+      <c r="M50" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="N4" s="31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="53" t="s">
-        <v>222</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="N50" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="63"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E51" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="F51" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="58" t="s">
+        <v>185</v>
+      </c>
+      <c r="I51" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" s="13" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="J51" s="11"/>
+      <c r="K51" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L51" s="33"/>
+      <c r="M51" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N51" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="O51" s="11"/>
+    </row>
+    <row r="52" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="63"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E52" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="F52" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G52" s="20"/>
+      <c r="H52" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="I52" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="32"/>
-      <c r="M6" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="N6" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" s="17" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="J52" s="20"/>
+      <c r="K52" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="L52" s="32"/>
+      <c r="M52" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N52" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="63"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="I7" s="17" t="s">
+      <c r="E53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="I53" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-    </row>
-    <row r="8" spans="1:25" s="13" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="J53" s="11"/>
+      <c r="K53" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L53" s="33"/>
+      <c r="M53" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N53" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="O53" s="11"/>
+    </row>
+    <row r="54" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="63"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="D54" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E54" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="I8" s="13" t="s">
+      <c r="F54" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="G54" s="20"/>
+      <c r="H54" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="I54" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="32"/>
-      <c r="M10" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="N11" s="33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="58" t="s">
-        <v>234</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="13" t="s">
+      <c r="J54" s="20"/>
+      <c r="K54" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="L54" s="32"/>
+      <c r="M54" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N54" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" s="17" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="N15" s="30"/>
-    </row>
-    <row r="16" spans="1:25" s="13" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="32"/>
-    </row>
-    <row r="17" spans="1:14" s="17" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="L17" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="M17" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="N17" s="30"/>
-    </row>
-    <row r="18" spans="1:14" s="13" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="M18" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="32"/>
-    </row>
-    <row r="19" spans="1:14" s="17" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="N19" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="13" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="N21" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="N22" s="32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="17" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="L23" s="30"/>
-      <c r="M23" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N23" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H24" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="L24" s="32"/>
-      <c r="M24" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="L25" s="30"/>
-      <c r="M25" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N25" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" s="58" t="s">
-        <v>149</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="L26" s="32"/>
-      <c r="M26" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="N26" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="I27" s="18"/>
-      <c r="K27" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="L27" s="30"/>
-      <c r="M27" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N27" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="42" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="H28" s="58" t="s">
-        <v>202</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="N28" s="31"/>
-    </row>
-    <row r="29" spans="1:14" s="21" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="20"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-    </row>
-    <row r="30" spans="1:14" s="17" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="N30" s="35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="M31" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N31" s="38"/>
-    </row>
-    <row r="32" spans="1:14" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="25"/>
-      <c r="K32" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="37"/>
-      <c r="M32" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="N32" s="39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="M33" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N33" s="38"/>
-    </row>
-    <row r="34" spans="1:15" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="61" t="s">
-        <v>156</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="N34" s="37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G35" s="16"/>
-      <c r="H35" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="M35" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N35" s="38"/>
-    </row>
-    <row r="36" spans="1:15" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="N36" s="37"/>
-    </row>
-    <row r="37" spans="1:15" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="H37" s="58"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-    </row>
-    <row r="38" spans="1:15" s="17" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="N38" s="35"/>
-    </row>
-    <row r="39" spans="1:15" s="13" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="16"/>
-      <c r="K39" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39" s="38"/>
-      <c r="M39" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="N39" s="36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="55"/>
-      <c r="C40" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G40" s="25"/>
-      <c r="H40" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J40" s="25"/>
-      <c r="K40" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40" s="37"/>
-      <c r="M40" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="N40" s="39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" s="13" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="16"/>
-      <c r="K41" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="N41" s="36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G42" s="25"/>
-      <c r="H42" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="M42" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N42" s="39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" s="13" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G43" s="16"/>
-      <c r="H43" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="M43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N43" s="36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" s="13" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="36"/>
-    </row>
-    <row r="45" spans="1:15" s="13" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="42"/>
-      <c r="H45" s="62"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-    </row>
-    <row r="46" spans="1:15" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="54"/>
-      <c r="C46" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G46" s="23"/>
-      <c r="H46" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="I46" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="N46" s="35"/>
-      <c r="O46" s="23"/>
-    </row>
-    <row r="47" spans="1:15" s="13" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="46" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="L47" s="38"/>
-      <c r="M47" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="N47" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="O47" s="16"/>
-    </row>
-    <row r="48" spans="1:15" s="17" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="G48" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H48" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="N48" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="O48" s="25"/>
-    </row>
-    <row r="49" spans="1:15" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J49" s="16"/>
-      <c r="K49" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="L49" s="38"/>
-      <c r="M49" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="N49" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="O49" s="16"/>
-    </row>
-    <row r="50" spans="1:15" s="17" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="G50" s="25"/>
-      <c r="H50" s="61" t="s">
-        <v>184</v>
-      </c>
-      <c r="I50" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J50" s="25"/>
-      <c r="K50" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="L50" s="37"/>
-      <c r="M50" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N50" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="O50" s="25"/>
-    </row>
-    <row r="51" spans="1:15" s="13" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="10"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G51" s="16"/>
-      <c r="H51" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="16"/>
-      <c r="K51" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="L51" s="38"/>
-      <c r="M51" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N51" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="O51" s="16"/>
-    </row>
-    <row r="52" spans="1:15" s="17" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="G52" s="25"/>
-      <c r="H52" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="I52" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="25"/>
-      <c r="K52" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="L52" s="37"/>
-      <c r="M52" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N52" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="O52" s="25"/>
-    </row>
-    <row r="53" spans="1:15" s="13" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="10"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="60" t="s">
-        <v>192</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="16"/>
-      <c r="K53" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="L53" s="38"/>
-      <c r="M53" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N53" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="O53" s="16"/>
-    </row>
-    <row r="54" spans="1:15" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="55"/>
-      <c r="C54" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="G54" s="25"/>
-      <c r="H54" s="61" t="s">
-        <v>196</v>
-      </c>
-      <c r="I54" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="25"/>
-      <c r="K54" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="L54" s="37"/>
-      <c r="M54" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N54" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="O54" s="25"/>
+      <c r="O54" s="20"/>
     </row>
     <row r="55" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="2"/>

</xml_diff>

<commit_message>
Write function Notification Options
Finished function showSettingsNotifications &
submitSettingsNotifications,  update Document Webservice and update plan
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="241">
   <si>
     <t>Header</t>
   </si>
@@ -1394,45 +1394,6 @@
 }</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>list_user_auto_pubishing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">: Lưu giá trị auto_pubishing lên các mạng xã hội (Facbook, Twitter, Tumblr)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>list_user_social_connection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>: Lưu giá trị On/Off tương tác với các mạng xã hội (Facbook, Twitter, FourSquare, Tumblr)</t>
-    </r>
-  </si>
-  <si>
     <t>USERS (SETTINGS)</t>
   </si>
   <si>
@@ -1664,184 +1625,6 @@
   </si>
   <si>
     <t>sender_id, recipient_id, message</t>
-  </si>
-  <si>
-    <t>get_options_value_notification</t>
-  </si>
-  <si>
-    <t>Lấy các tuỳ chọn đã được lưu ở mục Notification (trang Settings)</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/get_options_value_notification</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "list_user_notification_settings": [
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "y",
-                "@nsid": "1",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "y",
-                "@nsMobileFlag": "n",
-                "@nsid": "2",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "y",
-                "@nsMobileFlag": "n",
-                "@nsid": "3",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "4",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "5",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "6",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "7",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "8",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "9",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "10",
-                "@nsidType": "a",
-                "@userId": "1"
-            }
-        ],
-        "message": {
-            "code": 200,
-            "message": "Success"
-        }
-    }
-}</t>
-  </si>
-  <si>
-    <t>set_options_notification</t>
-  </si>
-  <si>
-    <t>Thiết lập các tuỳ chọn đã được lưu ở mục Notification (trang Settings)</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/set_options_notification</t>
-  </si>
-  <si>
-    <t>{
-    "notification_settings": {
-        "list_user_notification_settings": [
-            {
-                "@nsEmailFlag": "y",
-                "@nsMobileFlag": "n",
-                "@nsid": "1",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "y",
-                "@nsMobileFlag": "n",
-                "@nsid": "2",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "y",
-                "@nsMobileFlag": "n",
-                "@nsid": "3",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "4",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "5",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "6",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "7",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "8",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "9",
-                "@nsidType": "a",
-                "@userId": "1"
-            },
-            {
-                "@nsEmailFlag": "n",
-                "@nsMobileFlag": "n",
-                "@nsid": "10",
-                "@nsidType": "a",
-                "@userId": "1"
-            }
-        ]
-    }
-}</t>
   </si>
   <si>
     <t>get_options_value_about</t>
@@ -3624,59 +3407,73 @@
   </si>
   <si>
     <t>{
-    "user_log_id": "20130701171352-1-1-10",
-    "user": {
-        "autoUserId": "1",
-        "userId": "1-1",
-        "tsUserId": "1-1",
-        "tsUserEmail": "hphu90@gmail.com",
-        "tsUserPw": "abcde",
-        "tsFirstName": "Phan",
-        "tsLastName": "Phu",
-        "maxInvites": "100",
-        "userCreatedInitialDatetime": "",
-        "userPoints": "0",
-        "twitterUsrUrl": "",
-        "userDisabledFlag": "",
-        "userActivationKey": "",
-        "userGender": "",
-        "userCityId": "",
-        "userState": "",
-        "isOnline": "y",
-        "userCountry": "",
-        "about": "",
-        "currentStatus": "e",
-        "userFbId": ""
-    },
-    "user_profile_obj": null,
-    "user_data": null,
-    "city": null,
-    "fb_user_data": null,
-    "list_user_data": null,
-    "list_user": null,
-    "list_user_follow_data": null,
-    "list_fb_user_data": null,
-    "list_cities": null
-}</t>
-  </si>
-  <si>
-    <t>{
     "successMsg": "Logout success!"
 }</t>
   </si>
   <si>
+    <t>userLogId</t>
+  </si>
+  <si>
     <t>{
-    "user_log_id": "20130701180200-1-9-14",
+    "successMsg": "Settings success!"
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/settings/updateSettingsAutoPublishSettings</t>
+  </si>
+  <si>
+    <t>showSettingsSocial</t>
+  </si>
+  <si>
+    <t>submitOptionsAutoPublish</t>
+  </si>
+  <si>
+    <t>submitSettingsNotifications</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showSettingsNotifications</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/submitSettingsNotifications</t>
+  </si>
+  <si>
+    <t>showSettingsNotifications</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showSettingsSocial</t>
+  </si>
+  <si>
+    <t>Get user's options on Notification (page Settings)</t>
+  </si>
+  <si>
+    <t>Get user's options on Social Networks (page Settings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Set user's options on Social Networks (page Settings)</t>
+  </si>
+  <si>
+    <t>Set user's options on Notification (page Settings)</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "Settings Success!"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "user_log_id": "20130703173210-1-20130703173109-94728-46035",
     "user": {
-        "autoUserId": "9",
-        "userId": "1-9",
-        "tsUserId": "1-9",
+        "userId": "1-20130703173109-94728",
+        "tsUserId": "1-20130703173109-94728",
         "tsUserEmail": "tanhuu94_dn@gmail.com",
         "tsUserPw": "",
         "tsFirstName": "Phan",
         "tsLastName": "Huu",
         "maxInvites": "100",
-        "userCreatedInitialDatetime": "2013-06-28 09:51:16.0",
+        "userCreatedInitialDatetime": "2013-07-03 17:31:09.0",
         "userPoints": "0",
         "twitterUsrUrl": "",
         "userDisabledFlag": "",
@@ -3702,19 +3499,28 @@
 }</t>
   </si>
   <si>
-    <t>userLogId</t>
-  </si>
-  <si>
     <t>{
-    "successMsg": "Settings success!"
+    "userId": "1-20130703173109-94728",
+    "facebookStatus": "1",
+    "twitterStatus": "0",
+    "foursquareStatus": "0",
+    "tumblrStatus": "1",
+    "tsSocialAutoPubSettingsObj": {
+        "favFbFlag": "1",
+        "favTwitterFlag": "0",
+        "favTumblrFlag": "1",
+        "tipsFbFlag": "0",
+        "tipsTwitterFlag": "1",
+        "tipsTumblrFlag": "0",
+        "recoFbFlag": "1",
+        "recoTwitterFlag": "0",
+        "recoTumblrFlag": "1"
+    }
 }</t>
   </si>
   <si>
-    <t>http://localhost:8080/tsws/services/user/settings/updateSettingsAutoPublishSettings</t>
-  </si>
-  <si>
     <t>{
-    "email":"tanhuu94_dn@gmail.com",
+    "userId":"1-20130703173109-94728",
     "facebookStatus": "1",
     "twitterStatus": "1",
     "foursquareStatus": "0",
@@ -3733,34 +3539,102 @@
 }</t>
   </si>
   <si>
-    <t>showSettingsSocial</t>
-  </si>
-  <si>
-    <t>submitOptionsAutoPublish</t>
-  </si>
-  <si>
-    <t>Get user's options Social Networks (trang Settings)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Set user's options Social Networks (page Settings)</t>
-  </si>
-  <si>
     <t>{
-    "email": null,
-    "facebookStatus": "1",
-    "twitterStatus": "0",
-    "foursquareStatus": "0",
-    "tumblrStatus": "1",
-    "tsSocialAutoPubSettingsObj": {
-        "favFbFlag": "1",
-        "favTwitterFlag": "0",
-        "favTumblrFlag": "1",
-        "tipsFbFlag": "0",
-        "tipsTwitterFlag": "1",
-        "tipsTumblrFlag": "0",
-        "recoFbFlag": "1",
-        "recoTwitterFlag": "0",
-        "recoTumblrFlag": "1"
+    "userId":"1-20130703173109-94728",
+    "friendsAskReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "peopleFollowAskReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "otherPeopleAskReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "peopleLikeMyReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "peopleAskMeFollowReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "friendsSendMeReco":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "peopleLikeCommentTips":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "friendsPostQuestionForum":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "friendsJoinTasteSync":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    },
+    "newslettersDigestsTasteSync":
+    {
+ "phoneFlag":"1",
+ "emailFlag":"0"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "userId": "1-20130703173109-94728",
+    "friendsAskReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "peopleFollowAskReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "otherPeopleAskReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "peopleLikeMyReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "peopleAskMeFollowReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "friendsSendMeReco": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "peopleLikeCommentTips": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "friendsPostQuestionForum": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
+    },
+    "friendsJoinTasteSync": {
+        "phoneFlag": "1",
+        "emailFlag": "1"
+    },
+    "newslettersDigestsTasteSync": {
+        "phoneFlag": "1",
+        "emailFlag": "0"
     }
 }</t>
   </si>
@@ -3917,7 +3791,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4096,6 +3970,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4417,8 +4294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="H31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4444,28 +4321,28 @@
     <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:25" s="7" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H2" s="47" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>0</v>
@@ -4480,13 +4357,13 @@
         <v>3</v>
       </c>
       <c r="M2" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -4500,11 +4377,11 @@
       <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" s="12" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>4</v>
@@ -4516,32 +4393,32 @@
         <v>6</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="25"/>
       <c r="M3" s="28" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="44" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>23</v>
@@ -4553,30 +4430,30 @@
         <v>44</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="52" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="26" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="48" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>13</v>
@@ -4588,27 +4465,27 @@
         <v>6</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="L5" s="25"/>
       <c r="M5" s="28" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="44"/>
       <c r="C6" s="37" t="s">
         <v>9</v>
@@ -4620,10 +4497,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>7</v>
@@ -4633,14 +4510,14 @@
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="26" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="N6" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="48"/>
       <c r="C7" s="36" t="s">
         <v>15</v>
@@ -4655,7 +4532,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>7</v>
@@ -4668,7 +4545,7 @@
       <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:25" s="8" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="44"/>
       <c r="C8" s="37" t="s">
         <v>19</v>
@@ -4683,7 +4560,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>7</v>
@@ -4700,7 +4577,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="48"/>
       <c r="C9" s="36" t="s">
         <v>55</v>
@@ -4715,7 +4592,7 @@
         <v>56</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>7</v>
@@ -4732,7 +4609,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="44"/>
       <c r="C10" s="37" t="s">
         <v>59</v>
@@ -4747,7 +4624,7 @@
         <v>60</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>7</v>
@@ -4764,10 +4641,10 @@
       </c>
     </row>
     <row r="11" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="48"/>
       <c r="C11" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>5</v>
@@ -4776,10 +4653,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>7</v>
@@ -4789,14 +4666,14 @@
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="N11" s="28" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="12" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="44"/>
       <c r="C12" s="37" t="s">
         <v>61</v>
@@ -4814,7 +4691,7 @@
         <v>93</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>7</v>
@@ -4831,7 +4708,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="48"/>
       <c r="C13" s="36" t="s">
         <v>66</v>
@@ -4849,7 +4726,7 @@
         <v>93</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>7</v>
@@ -4866,7 +4743,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="44"/>
       <c r="C14" s="37" t="s">
         <v>74</v>
@@ -4898,7 +4775,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" s="12" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="48"/>
       <c r="C15" s="36" t="s">
         <v>77</v>
@@ -4923,7 +4800,7 @@
       <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="44"/>
       <c r="C16" s="37" t="s">
         <v>81</v>
@@ -4952,7 +4829,7 @@
       <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" s="12" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="48"/>
       <c r="C17" s="36" t="s">
         <v>85</v>
@@ -4979,7 +4856,7 @@
         <v>94</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="M17" s="25" t="s">
         <v>65</v>
@@ -4987,7 +4864,7 @@
       <c r="N17" s="25"/>
     </row>
     <row r="18" spans="1:14" s="8" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="44"/>
       <c r="C18" s="37" t="s">
         <v>88</v>
@@ -5011,7 +4888,7 @@
         <v>47</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="M18" s="26" t="s">
         <v>49</v>
@@ -5019,7 +4896,7 @@
       <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" s="12" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="48"/>
       <c r="C19" s="36" t="s">
         <v>95</v>
@@ -5047,14 +4924,14 @@
       </c>
       <c r="L19" s="28"/>
       <c r="M19" s="28" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="N19" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="44"/>
       <c r="C20" s="37" t="s">
         <v>98</v>
@@ -5087,7 +4964,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="48"/>
       <c r="C21" s="36" t="s">
         <v>103</v>
@@ -5119,7 +4996,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="44"/>
       <c r="C22" s="37" t="s">
         <v>107</v>
@@ -5151,10 +5028,10 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="12" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="48"/>
       <c r="C23" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>5</v>
@@ -5163,19 +5040,19 @@
         <v>6</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>7</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="28" t="s">
@@ -5186,10 +5063,10 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="44"/>
       <c r="C24" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>5</v>
@@ -5198,16 +5075,16 @@
         <v>6</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="26" t="s">
@@ -5218,10 +5095,10 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="48"/>
       <c r="C25" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>5</v>
@@ -5230,16 +5107,16 @@
         <v>6</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="22" t="s">
         <v>133</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>134</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>7</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="28" t="s">
@@ -5250,10 +5127,10 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="44"/>
       <c r="C26" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>5</v>
@@ -5262,30 +5139,30 @@
         <v>6</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H26" s="53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" s="27"/>
       <c r="M26" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N26" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="48"/>
       <c r="C27" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>5</v>
@@ -5294,14 +5171,14 @@
         <v>6</v>
       </c>
       <c r="F27" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="22" t="s">
         <v>141</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>142</v>
       </c>
       <c r="I27" s="13"/>
       <c r="K27" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="28" t="s">
@@ -5312,27 +5189,27 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="44"/>
       <c r="C28" s="37" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H28" s="53" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L28" s="27"/>
       <c r="M28" s="26" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="N28" s="26"/>
     </row>
@@ -5349,14 +5226,14 @@
       <c r="N29" s="29"/>
     </row>
     <row r="30" spans="1:14" s="12" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="61" t="s">
-        <v>112</v>
+      <c r="A30" s="62" t="s">
+        <v>111</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>5</v>
@@ -5365,34 +5242,32 @@
         <v>6</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>111</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="G30" s="17"/>
       <c r="H30" s="54" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J30" s="18"/>
       <c r="K30" s="18" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="L30" s="30"/>
       <c r="M30" s="30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N30" s="30"/>
     </row>
     <row r="31" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="62"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="46" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>5</v>
@@ -5401,11 +5276,11 @@
         <v>44</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="59" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>47</v>
@@ -5413,20 +5288,20 @@
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
       <c r="L31" s="31" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="62"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="50"/>
       <c r="C32" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>5</v>
@@ -5435,11 +5310,11 @@
         <v>6</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>7</v>
@@ -5450,17 +5325,17 @@
       </c>
       <c r="L32" s="32"/>
       <c r="M32" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N32" s="34" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="62"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="46"/>
       <c r="C33" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>5</v>
@@ -5469,11 +5344,11 @@
         <v>44</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>47</v>
@@ -5481,7 +5356,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M33" s="31" t="s">
         <v>49</v>
@@ -5489,10 +5364,12 @@
       <c r="N33" s="33"/>
     </row>
     <row r="34" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="62"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="50" t="s">
+        <v>203</v>
+      </c>
       <c r="C34" s="42" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>5</v>
@@ -5501,32 +5378,32 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="G34" s="20"/>
-      <c r="H34" s="56" t="s">
-        <v>146</v>
+      <c r="H34" s="60" t="s">
+        <v>227</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="20" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="L34" s="32"/>
       <c r="M34" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="N34" s="32" t="s">
-        <v>65</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="N34" s="32"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="62"/>
-      <c r="B35" s="46"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="46" t="s">
+        <v>203</v>
+      </c>
       <c r="C35" s="41" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>5</v>
@@ -5535,11 +5412,11 @@
         <v>44</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>149</v>
+        <v>234</v>
       </c>
       <c r="G35" s="11"/>
-      <c r="H35" s="55" t="s">
-        <v>150</v>
+      <c r="H35" s="59" t="s">
+        <v>228</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>47</v>
@@ -5547,29 +5424,31 @@
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
       <c r="L35" s="31" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="N35" s="33"/>
+        <v>235</v>
+      </c>
+      <c r="N35" s="26" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="36" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="62"/>
+      <c r="A36" s="63"/>
       <c r="B36" s="50"/>
       <c r="C36" s="42" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>25</v>
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="19" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="56" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>7</v>
@@ -5578,7 +5457,7 @@
       <c r="K36" s="20"/>
       <c r="L36" s="32"/>
       <c r="M36" s="34" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="N36" s="32"/>
     </row>
@@ -5594,7 +5473,7 @@
       <c r="N37" s="27"/>
     </row>
     <row r="38" spans="1:15" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="64" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="49"/>
@@ -5619,12 +5498,12 @@
       <c r="K38" s="18"/>
       <c r="L38" s="30"/>
       <c r="M38" s="30" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="N38" s="30"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="64"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="46"/>
       <c r="C39" s="41" t="s">
         <v>33</v>
@@ -5658,7 +5537,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="64"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="50"/>
       <c r="C40" s="42" t="s">
         <v>35</v>
@@ -5692,7 +5571,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="64"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="46"/>
       <c r="C41" s="41" t="s">
         <v>36</v>
@@ -5726,7 +5605,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="64"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="50"/>
       <c r="C42" s="42" t="s">
         <v>43</v>
@@ -5760,7 +5639,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="64"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="46"/>
       <c r="C43" s="41" t="s">
         <v>51</v>
@@ -5794,7 +5673,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="64"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="46"/>
       <c r="C44" s="41"/>
       <c r="D44" s="10"/>
@@ -5819,7 +5698,7 @@
       <c r="N45" s="27"/>
     </row>
     <row r="46" spans="1:15" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>68</v>
       </c>
       <c r="B46" s="49"/>
@@ -5850,10 +5729,10 @@
       <c r="O46" s="18"/>
     </row>
     <row r="47" spans="1:15" s="8" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="64"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="46"/>
       <c r="C47" s="41" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>5</v>
@@ -5862,24 +5741,24 @@
         <v>6</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>93</v>
       </c>
       <c r="H47" s="55" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="I47" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J47" s="11"/>
       <c r="K47" s="11" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="31" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="N47" s="33" t="s">
         <v>65</v>
@@ -5887,10 +5766,10 @@
       <c r="O47" s="11"/>
     </row>
     <row r="48" spans="1:15" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="64"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="50"/>
       <c r="C48" s="42" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>5</v>
@@ -5899,24 +5778,24 @@
         <v>6</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>93</v>
       </c>
       <c r="H48" s="56" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I48" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J48" s="20"/>
       <c r="K48" s="20" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="L48" s="32"/>
       <c r="M48" s="32" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="N48" s="32" t="s">
         <v>65</v>
@@ -5924,10 +5803,10 @@
       <c r="O48" s="20"/>
     </row>
     <row r="49" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="64"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="46"/>
       <c r="C49" s="41" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>5</v>
@@ -5936,22 +5815,22 @@
         <v>6</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="55" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I49" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J49" s="11"/>
       <c r="K49" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="31" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="N49" s="31" t="s">
         <v>65</v>
@@ -5959,10 +5838,10 @@
       <c r="O49" s="11"/>
     </row>
     <row r="50" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="64"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="50"/>
       <c r="C50" s="42" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>5</v>
@@ -5971,18 +5850,18 @@
         <v>6</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G50" s="20"/>
       <c r="H50" s="56" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J50" s="20"/>
       <c r="K50" s="19" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L50" s="32"/>
       <c r="M50" s="34" t="s">
@@ -5994,10 +5873,10 @@
       <c r="O50" s="20"/>
     </row>
     <row r="51" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="64"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="46"/>
       <c r="C51" s="41" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>5</v>
@@ -6006,18 +5885,18 @@
         <v>6</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="58" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I51" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J51" s="11"/>
       <c r="K51" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="31" t="s">
@@ -6029,10 +5908,10 @@
       <c r="O51" s="11"/>
     </row>
     <row r="52" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="64"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="50"/>
       <c r="C52" s="42" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>5</v>
@@ -6041,18 +5920,18 @@
         <v>6</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="56" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I52" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J52" s="20"/>
       <c r="K52" s="19" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L52" s="32"/>
       <c r="M52" s="34" t="s">
@@ -6064,10 +5943,10 @@
       <c r="O52" s="20"/>
     </row>
     <row r="53" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="64"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="46"/>
       <c r="C53" s="41" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>5</v>
@@ -6076,18 +5955,18 @@
         <v>6</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="55" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I53" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J53" s="11"/>
       <c r="K53" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="31" t="s">
@@ -6099,10 +5978,10 @@
       <c r="O53" s="11"/>
     </row>
     <row r="54" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="64"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="50"/>
       <c r="C54" s="42" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>5</v>
@@ -6111,18 +5990,18 @@
         <v>6</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G54" s="20"/>
       <c r="H54" s="56" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J54" s="20"/>
       <c r="K54" s="19" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="L54" s="32"/>
       <c r="M54" s="34" t="s">

</xml_diff>

<commit_message>
Write function Contact and About
Contact & About menu. Fix all setting with order colum. Update plan and
fix API_Webservice
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="243">
   <si>
     <t>Header</t>
   </si>
@@ -1493,59 +1493,6 @@
     <t>sender_id, recipient_id, message</t>
   </si>
   <si>
-    <t>get_options_value_about</t>
-  </si>
-  <si>
-    <t>Lấy các nội dung trong mục About (FAQ, Privacy Policy….)</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/get_options_value_about</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "list_about_tastesync_descriptor": [
-            {
-                "@created": "2013-04-04 00:00:00.0",
-                "@description": "Test for Frequently Asked Questions",
-                "@id": "1",
-                "@idOrder": "1",
-                "@name": "Frequently Asked Questions",
-                "@usgId": "6"
-            },
-            {
-                "@created": "2013-04-04 00:00:00.0",
-                "@description": "Test for Terms of Service",
-                "@id": "2",
-                "@idOrder": "2",
-                "@name": "Terms of Service",
-                "@usgId": "6"
-            },
-            {
-                "@created": "2013-04-04 00:00:00.0",
-                "@description": "Test for Privacy Policy",
-                "@id": "3",
-                "@idOrder": "3",
-                "@name": "Privacy Policy",
-                "@usgId": "6"
-            },
-            {
-                "@created": "2013-04-04 00:00:00.0",
-                "@description": "Test for Attribution",
-                "@id": "4",
-                "@idOrder": "4",
-                "@name": "Attribution",
-                "@usgId": "6"
-            }
-        ],
-        "message": {
-            "code": 200,
-            "message": "Success"
-        }
-    }
-}</t>
-  </si>
-  <si>
     <t>get_list_restaurants_when_wait_for</t>
   </si>
   <si>
@@ -3291,9 +3238,6 @@
     <t>showSettingsSocial</t>
   </si>
   <si>
-    <t>submitOptionsAutoPublish</t>
-  </si>
-  <si>
     <t>submitSettingsNotifications</t>
   </si>
   <si>
@@ -3362,46 +3306,6 @@
     "list_user_follow_data": null,
     "list_fb_user_data": null,
     "list_cities": null
-}</t>
-  </si>
-  <si>
-    <t>{
-    "userId": "1-20130703173109-94728",
-    "facebookStatus": "1",
-    "twitterStatus": "0",
-    "foursquareStatus": "0",
-    "tumblrStatus": "1",
-    "tsSocialAutoPubSettingsObj": {
-        "favFbFlag": "1",
-        "favTwitterFlag": "0",
-        "favTumblrFlag": "1",
-        "tipsFbFlag": "0",
-        "tipsTwitterFlag": "1",
-        "tipsTumblrFlag": "0",
-        "recoFbFlag": "1",
-        "recoTwitterFlag": "0",
-        "recoTumblrFlag": "1"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "userId":"1-20130703173109-94728",
-    "facebookStatus": "1",
-    "twitterStatus": "1",
-    "foursquareStatus": "0",
-    "tumblrStatus": "1",
-    "tsSocialAutoPubSettingsObj": {
-        "favFbFlag": "1",
-        "favTwitterFlag": "0",
-        "favTumblrFlag": "1",
-        "tipsFbFlag": "1",
-        "tipsTwitterFlag": "1",
-        "tipsTumblrFlag": "0",
-        "recoFbFlag": "0",
-        "recoTwitterFlag": "0",
-        "recoTumblrFlag": "1"
-    }
 }</t>
   </si>
   <si>
@@ -3517,6 +3421,123 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>{
+    "userId": "1-20130703173109-94728",
+    "socialSettings": [
+        {
+            "usncORDER": "1",
+            "usncYN": "1",
+            "auto_publishing": [
+                {
+                    "usncORDER": "1",
+                    "usncYN": "1"
+                },
+                {
+                    "usncORDER": "2",
+                    "usncYN": "1"
+                },
+                {
+                    "usncORDER": "3",
+                    "usncYN": "0"
+                }
+            ]
+        },
+        {
+            "usncORDER": "2",
+            "usncYN": "1",
+            "auto_publishing": [
+                {
+                    "usncORDER": "1",
+                    "usncYN": "1"
+                },
+                {
+                    "usncORDER": "2",
+                    "usncYN": "1"
+                },
+                {
+                    "usncORDER": "3",
+                    "usncYN": "0"
+                }
+            ]
+        },
+        {
+            "usncORDER": "3",
+            "usncYN": "1",
+            "auto_publishing": [
+                null,
+                null,
+                null
+            ]
+        },
+        {
+            "usncORDER": "4",
+            "usncYN": "1",
+            "auto_publishing": [
+                {
+                    "usncORDER": "1",
+                    "usncYN": "1"
+                },
+                {
+                    "usncORDER": "2",
+                    "usncYN": "0"
+                },
+                {
+                    "usncORDER": "3",
+                    "usncYN": "1"
+                }
+            ]
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>submitSettingsSocial</t>
+  </si>
+  <si>
+    <t>showAboutTastesync</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>submitSettingscontactUs</t>
+  </si>
+  <si>
+    <t>userId, Contact_Order, Contact_Desc</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/submitSettingsContactUs</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showAboutTastesync</t>
+  </si>
+  <si>
+    <t>Get content of About menu (FAQ, Privacy Policy….)</t>
+  </si>
+  <si>
+    <t>Submit feedback to server</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "order": "1",
+        "content": "Test for Frequently Asked Questions"
+    },
+    {
+        "order": "2",
+        "content": "Test for Terms of Service"
+    },
+    {
+        "order": "3",
+        "content": "Test for Privacy Policy"
+    },
+    {
+        "order": "4",
+        "content": "Test for Attribution"
+    }
+]</t>
   </si>
 </sst>
 </file>
@@ -3671,7 +3692,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3854,6 +3875,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -4172,10 +4196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y131"/>
+  <dimension ref="A1:Y132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="I28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4201,28 +4225,28 @@
     <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:25" s="7" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="G2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="H2" s="47" t="s">
         <v>183</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>187</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>0</v>
@@ -4237,13 +4261,13 @@
         <v>3</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -4257,11 +4281,11 @@
       <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" s="12" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>4</v>
@@ -4273,32 +4297,32 @@
         <v>6</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="25"/>
       <c r="M3" s="28" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="44" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>23</v>
@@ -4310,30 +4334,30 @@
         <v>44</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="52" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="48" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>13</v>
@@ -4345,27 +4369,27 @@
         <v>6</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L5" s="25"/>
       <c r="M5" s="28" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="44"/>
       <c r="C6" s="37" t="s">
         <v>9</v>
@@ -4377,10 +4401,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>7</v>
@@ -4390,14 +4414,14 @@
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="26" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="N6" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="48"/>
       <c r="C7" s="36" t="s">
         <v>15</v>
@@ -4412,7 +4436,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>7</v>
@@ -4425,7 +4449,7 @@
       <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:25" s="8" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="44"/>
       <c r="C8" s="37" t="s">
         <v>19</v>
@@ -4440,7 +4464,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>7</v>
@@ -4457,7 +4481,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="48"/>
       <c r="C9" s="36" t="s">
         <v>55</v>
@@ -4472,7 +4496,7 @@
         <v>56</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>7</v>
@@ -4489,7 +4513,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="44"/>
       <c r="C10" s="37" t="s">
         <v>59</v>
@@ -4504,7 +4528,7 @@
         <v>60</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>7</v>
@@ -4521,7 +4545,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="48"/>
       <c r="C11" s="36" t="s">
         <v>112</v>
@@ -4536,7 +4560,7 @@
         <v>113</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>7</v>
@@ -4553,7 +4577,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="44"/>
       <c r="C12" s="37" t="s">
         <v>61</v>
@@ -4571,7 +4595,7 @@
         <v>93</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>7</v>
@@ -4588,7 +4612,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="48"/>
       <c r="C13" s="36" t="s">
         <v>66</v>
@@ -4606,7 +4630,7 @@
         <v>93</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>7</v>
@@ -4623,7 +4647,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="44"/>
       <c r="C14" s="37" t="s">
         <v>74</v>
@@ -4655,7 +4679,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" s="12" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="48"/>
       <c r="C15" s="36" t="s">
         <v>77</v>
@@ -4680,7 +4704,7 @@
       <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="44"/>
       <c r="C16" s="37" t="s">
         <v>81</v>
@@ -4709,7 +4733,7 @@
       <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" s="12" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="48"/>
       <c r="C17" s="36" t="s">
         <v>85</v>
@@ -4736,7 +4760,7 @@
         <v>94</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M17" s="25" t="s">
         <v>65</v>
@@ -4744,7 +4768,7 @@
       <c r="N17" s="25"/>
     </row>
     <row r="18" spans="1:14" s="8" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="61"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="44"/>
       <c r="C18" s="37" t="s">
         <v>88</v>
@@ -4768,7 +4792,7 @@
         <v>47</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M18" s="26" t="s">
         <v>49</v>
@@ -4776,7 +4800,7 @@
       <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" s="12" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="61"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="48"/>
       <c r="C19" s="36" t="s">
         <v>95</v>
@@ -4804,14 +4828,14 @@
       </c>
       <c r="L19" s="28"/>
       <c r="M19" s="28" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="N19" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="61"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="44"/>
       <c r="C20" s="37" t="s">
         <v>98</v>
@@ -4844,7 +4868,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="61"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="48"/>
       <c r="C21" s="36" t="s">
         <v>103</v>
@@ -4876,7 +4900,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="61"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="44"/>
       <c r="C22" s="37" t="s">
         <v>107</v>
@@ -4908,7 +4932,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="12" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="48"/>
       <c r="C23" s="36" t="s">
         <v>116</v>
@@ -4923,7 +4947,7 @@
         <v>117</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H23" s="22" t="s">
         <v>118</v>
@@ -4943,7 +4967,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="61"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="44"/>
       <c r="C24" s="37" t="s">
         <v>120</v>
@@ -4975,7 +4999,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="61"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="48"/>
       <c r="C25" s="36" t="s">
         <v>123</v>
@@ -5007,7 +5031,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="61"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="44"/>
       <c r="C26" s="37" t="s">
         <v>127</v>
@@ -5039,7 +5063,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="48"/>
       <c r="C27" s="36" t="s">
         <v>131</v>
@@ -5069,27 +5093,27 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="61"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="44"/>
       <c r="C28" s="37" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H28" s="53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L28" s="27"/>
       <c r="M28" s="26" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="N28" s="26"/>
     </row>
@@ -5106,14 +5130,14 @@
       <c r="N29" s="29"/>
     </row>
     <row r="30" spans="1:14" s="12" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="63" t="s">
         <v>111</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>5</v>
@@ -5122,32 +5146,32 @@
         <v>6</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="54" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J30" s="18"/>
       <c r="K30" s="18" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L30" s="30"/>
       <c r="M30" s="30" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="N30" s="30"/>
     </row>
     <row r="31" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="63"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="46" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>5</v>
@@ -5156,11 +5180,11 @@
         <v>44</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="59" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>47</v>
@@ -5168,22 +5192,22 @@
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
       <c r="L31" s="31" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>5</v>
@@ -5192,32 +5216,32 @@
         <v>6</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="56" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
       <c r="J32" s="20"/>
       <c r="K32" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L32" s="32"/>
       <c r="M32" s="34" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="N32" s="34"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="46" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>5</v>
@@ -5226,11 +5250,11 @@
         <v>44</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="55" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>47</v>
@@ -5238,22 +5262,22 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="31" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N33" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="63"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>5</v>
@@ -5262,32 +5286,32 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="60" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L34" s="32"/>
       <c r="M34" s="32" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="N34" s="32"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="46" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>5</v>
@@ -5296,11 +5320,11 @@
         <v>44</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="59" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>47</v>
@@ -5308,596 +5332,633 @@
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
       <c r="L35" s="31" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="N35" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="50" t="s">
+        <v>235</v>
+      </c>
       <c r="C36" s="42" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="F36" s="19" t="s">
-        <v>136</v>
+        <v>241</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="56" t="s">
-        <v>137</v>
+        <v>238</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
       <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="K36" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="L36" s="32"/>
       <c r="M36" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="N36" s="32"/>
+        <v>222</v>
+      </c>
+      <c r="N36" s="32" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="H37" s="53"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-    </row>
-    <row r="38" spans="1:15" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="64" t="s">
+      <c r="A37" s="61"/>
+      <c r="B37" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="N37" s="33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="H38" s="53"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+    </row>
+    <row r="39" spans="1:15" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="40" t="s">
+      <c r="B39" s="49"/>
+      <c r="C39" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D39" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18" t="s">
+      <c r="E39" s="18"/>
+      <c r="F39" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="18"/>
-      <c r="H38" s="54" t="s">
+      <c r="G39" s="18"/>
+      <c r="H39" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I39" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="N38" s="30"/>
-    </row>
-    <row r="39" spans="1:15" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="65"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="41" t="s">
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="N39" s="30"/>
+    </row>
+    <row r="40" spans="1:15" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="66"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="55" t="s">
+      <c r="G40" s="11"/>
+      <c r="H40" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I40" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="10" t="s">
+      <c r="J40" s="11"/>
+      <c r="K40" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L39" s="33"/>
-      <c r="M39" s="31" t="s">
+      <c r="L40" s="33"/>
+      <c r="M40" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="N39" s="31" t="s">
+      <c r="N40" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="65"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="42" t="s">
+    <row r="41" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="66"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E41" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F41" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="56" t="s">
+      <c r="G41" s="20"/>
+      <c r="H41" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="I41" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="19" t="s">
+      <c r="J41" s="20"/>
+      <c r="K41" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="32"/>
-      <c r="M40" s="34" t="s">
+      <c r="L41" s="32"/>
+      <c r="M41" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="N40" s="34" t="s">
+      <c r="N41" s="34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="65"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="41" t="s">
+    <row r="42" spans="1:15" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="66"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="55" t="s">
+      <c r="G42" s="11"/>
+      <c r="H42" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="11" t="s">
+      <c r="I42" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J41" s="11"/>
-      <c r="K41" s="10" t="s">
+      <c r="J42" s="11"/>
+      <c r="K42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33" t="s">
+      <c r="L42" s="33"/>
+      <c r="M42" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="N41" s="31" t="s">
+      <c r="N42" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="65"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="42" t="s">
+    <row r="43" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="66"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D43" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E43" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F43" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="56" t="s">
+      <c r="G43" s="20"/>
+      <c r="H43" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="I42" s="19" t="s">
+      <c r="I43" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="34" t="s">
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="M42" s="34" t="s">
+      <c r="M43" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N42" s="34" t="s">
+      <c r="N43" s="34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="65"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="41" t="s">
+    <row r="44" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="66"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="55" t="s">
+      <c r="G44" s="11"/>
+      <c r="H44" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="I43" s="10" t="s">
+      <c r="I44" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="M43" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="N43" s="31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="65"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="10"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-    </row>
-    <row r="45" spans="1:15" s="8" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="37"/>
-      <c r="H45" s="57"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-    </row>
-    <row r="46" spans="1:15" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="64" t="s">
+      <c r="L44" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M44" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N44" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="66"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+    </row>
+    <row r="46" spans="1:15" s="8" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="37"/>
+      <c r="H46" s="57"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+    </row>
+    <row r="47" spans="1:15" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="49"/>
-      <c r="C46" s="40" t="s">
+      <c r="B47" s="49"/>
+      <c r="C47" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D47" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="17" t="s">
+      <c r="E47" s="18"/>
+      <c r="F47" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="18"/>
-      <c r="H46" s="54" t="s">
+      <c r="G47" s="18"/>
+      <c r="H47" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I47" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="35" t="s">
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="N46" s="30"/>
-      <c r="O46" s="18"/>
-    </row>
-    <row r="47" spans="1:15" s="8" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="65"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="41" t="s">
+      <c r="N47" s="30"/>
+      <c r="O47" s="18"/>
+    </row>
+    <row r="48" spans="1:15" s="8" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="66"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="L48" s="33"/>
+      <c r="M48" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="N48" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="O48" s="11"/>
+    </row>
+    <row r="49" spans="1:15" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="66"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D49" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E49" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F49" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="G47" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H47" s="55" t="s">
-        <v>140</v>
-      </c>
-      <c r="I47" s="10" t="s">
+      <c r="N49" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="66"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G50" s="11"/>
+      <c r="H50" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="I50" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="L47" s="33"/>
-      <c r="M47" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="N47" s="33" t="s">
+      <c r="J50" s="11"/>
+      <c r="K50" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L50" s="33"/>
+      <c r="M50" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="N50" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="O47" s="11"/>
-    </row>
-    <row r="48" spans="1:15" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="65"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="D48" s="19" t="s">
+      <c r="O50" s="11"/>
+    </row>
+    <row r="51" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="66"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E51" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H48" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" s="19" t="s">
+      <c r="F51" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G51" s="20"/>
+      <c r="H51" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="I51" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32" t="s">
+      <c r="J51" s="20"/>
+      <c r="K51" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="L51" s="32"/>
+      <c r="M51" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N51" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="O48" s="20"/>
-    </row>
-    <row r="49" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="65"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="O51" s="20"/>
+    </row>
+    <row r="52" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="66"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="I49" s="10" t="s">
+      <c r="F52" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="H52" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="I52" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J49" s="11"/>
-      <c r="K49" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="L49" s="33"/>
-      <c r="M49" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="N49" s="31" t="s">
+      <c r="J52" s="11"/>
+      <c r="K52" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L52" s="33"/>
+      <c r="M52" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N52" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="O49" s="11"/>
-    </row>
-    <row r="50" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="65"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="D50" s="19" t="s">
+      <c r="O52" s="11"/>
+    </row>
+    <row r="53" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="66"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E53" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="I50" s="19" t="s">
+      <c r="F53" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G53" s="20"/>
+      <c r="H53" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="I53" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J50" s="20"/>
-      <c r="K50" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="L50" s="32"/>
-      <c r="M50" s="34" t="s">
+      <c r="J53" s="20"/>
+      <c r="K53" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="L53" s="32"/>
+      <c r="M53" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N50" s="34" t="s">
+      <c r="N53" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="O50" s="20"/>
-    </row>
-    <row r="51" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="65"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="66"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="G51" s="11"/>
-      <c r="H51" s="58" t="s">
+      <c r="F54" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="G54" s="11"/>
+      <c r="H54" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="I54" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J51" s="11"/>
-      <c r="K51" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="L51" s="33"/>
-      <c r="M51" s="31" t="s">
+      <c r="J54" s="11"/>
+      <c r="K54" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L54" s="33"/>
+      <c r="M54" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="N51" s="31" t="s">
+      <c r="N54" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="O51" s="11"/>
-    </row>
-    <row r="52" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="65"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" s="19" t="s">
+      <c r="O54" s="11"/>
+    </row>
+    <row r="55" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="66"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E55" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="56" t="s">
-        <v>163</v>
-      </c>
-      <c r="I52" s="19" t="s">
+      <c r="F55" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="20"/>
+      <c r="H55" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="I55" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J52" s="20"/>
-      <c r="K52" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="L52" s="32"/>
-      <c r="M52" s="34" t="s">
+      <c r="J55" s="20"/>
+      <c r="K55" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="L55" s="32"/>
+      <c r="M55" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N52" s="34" t="s">
+      <c r="N55" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="O52" s="20"/>
-    </row>
-    <row r="53" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="65"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="55" t="s">
-        <v>165</v>
-      </c>
-      <c r="I53" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="11"/>
-      <c r="K53" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="L53" s="33"/>
-      <c r="M53" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="N53" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="O53" s="11"/>
-    </row>
-    <row r="54" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="65"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="56" t="s">
-        <v>169</v>
-      </c>
-      <c r="I54" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="20"/>
-      <c r="K54" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="L54" s="32"/>
-      <c r="M54" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="N54" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="O54" s="20"/>
-    </row>
-    <row r="55" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="2"/>
+      <c r="O55" s="20"/>
     </row>
     <row r="56" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D56" s="2"/>
@@ -6126,29 +6187,32 @@
     </row>
     <row r="131" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D132" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:A28"/>
     <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A46:A54"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1"/>
     <hyperlink ref="H5" r:id="rId2"/>
     <hyperlink ref="H8" r:id="rId3"/>
-    <hyperlink ref="H38" r:id="rId4"/>
-    <hyperlink ref="H39" r:id="rId5"/>
-    <hyperlink ref="H40" r:id="rId6"/>
-    <hyperlink ref="H41" r:id="rId7"/>
-    <hyperlink ref="H42" r:id="rId8"/>
-    <hyperlink ref="H43" r:id="rId9"/>
+    <hyperlink ref="H39" r:id="rId4"/>
+    <hyperlink ref="H40" r:id="rId5"/>
+    <hyperlink ref="H41" r:id="rId6"/>
+    <hyperlink ref="H42" r:id="rId7"/>
+    <hyperlink ref="H43" r:id="rId8"/>
+    <hyperlink ref="H44" r:id="rId9"/>
     <hyperlink ref="H9" r:id="rId10"/>
     <hyperlink ref="H10" r:id="rId11"/>
     <hyperlink ref="H12" r:id="rId12"/>
     <hyperlink ref="H13" r:id="rId13"/>
-    <hyperlink ref="H46" r:id="rId14"/>
+    <hyperlink ref="H47" r:id="rId14"/>
     <hyperlink ref="H14" r:id="rId15"/>
     <hyperlink ref="H15" r:id="rId16"/>
     <hyperlink ref="H16" r:id="rId17"/>
@@ -6166,18 +6230,18 @@
     <hyperlink ref="H27" r:id="rId29"/>
     <hyperlink ref="H34" r:id="rId30"/>
     <hyperlink ref="H35" r:id="rId31"/>
-    <hyperlink ref="H36" r:id="rId32"/>
-    <hyperlink ref="H47" r:id="rId33"/>
-    <hyperlink ref="H48" r:id="rId34"/>
-    <hyperlink ref="H49" r:id="rId35"/>
-    <hyperlink ref="H50" r:id="rId36"/>
-    <hyperlink ref="H52" r:id="rId37"/>
-    <hyperlink ref="H53" r:id="rId38"/>
-    <hyperlink ref="H54" r:id="rId39"/>
-    <hyperlink ref="H28" r:id="rId40"/>
-    <hyperlink ref="H7" r:id="rId41"/>
-    <hyperlink ref="H3" r:id="rId42"/>
-    <hyperlink ref="H4" r:id="rId43"/>
+    <hyperlink ref="H48" r:id="rId32"/>
+    <hyperlink ref="H49" r:id="rId33"/>
+    <hyperlink ref="H50" r:id="rId34"/>
+    <hyperlink ref="H51" r:id="rId35"/>
+    <hyperlink ref="H53" r:id="rId36"/>
+    <hyperlink ref="H54" r:id="rId37"/>
+    <hyperlink ref="H55" r:id="rId38"/>
+    <hyperlink ref="H28" r:id="rId39"/>
+    <hyperlink ref="H7" r:id="rId40"/>
+    <hyperlink ref="H3" r:id="rId41"/>
+    <hyperlink ref="H4" r:id="rId42"/>
+    <hyperlink ref="H37" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId44"/>

</xml_diff>

<commit_message>
Submit Friend and Follow Friend
Create new API submitFollowUserStatusChange + showFollowStatus +
submitTrustedFriendStatusChange+ showTrustedFriend. Update plan. Add
document webservices
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="248">
   <si>
     <t>Header</t>
   </si>
@@ -1318,25 +1318,7 @@
     <t>user_id, contact_id, message</t>
   </si>
   <si>
-    <t>add_friend</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/add_friend</t>
-  </si>
-  <si>
     <t>user_id, friend_id</t>
-  </si>
-  <si>
-    <t>remove_friend</t>
-  </si>
-  <si>
-    <t>Thêm bạn vào danh sách bạn bè trên TasteSync</t>
-  </si>
-  <si>
-    <t>Loại bạn ra khỏi  danh sách bạn bè trên TasteSync</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/remove_friend</t>
   </si>
   <si>
     <t>check_friend</t>
@@ -3598,6 +3580,43 @@
         "create": null
     }
 ]</t>
+  </si>
+  <si>
+    <t>showTrustedFriend</t>
+  </si>
+  <si>
+    <t>submitTrustedFriendStatusChange</t>
+  </si>
+  <si>
+    <t>Show status friend on TasteSync</t>
+  </si>
+  <si>
+    <t>Add new friend on TasteSync</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showTrustedFriend</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/submitTrustedFriendStatusChange</t>
+  </si>
+  <si>
+    <t>userId, destUserId, trustedFriendStatus</t>
+  </si>
+  <si>
+    <t>userId, destUserId</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "not trust"
+}
+OR
+{
+    "successMsg": "trusted"
+}
+OR
+{
+    "successMsg": "no friend"
+}</t>
   </si>
 </sst>
 </file>
@@ -3752,20 +3771,8 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3819,12 +3826,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3861,30 +3862,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -3906,38 +3883,56 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -4256,1999 +4251,1737 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y132"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1"/>
-    <col min="2" max="2" width="8" style="43" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="3"/>
-    <col min="5" max="5" width="34" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="46.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="43.5703125" style="51" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="2"/>
-    <col min="10" max="10" width="17.140625" style="4"/>
-    <col min="11" max="11" width="30.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" style="23" customWidth="1"/>
-    <col min="13" max="13" width="56.42578125" style="23" customWidth="1"/>
-    <col min="14" max="14" width="41.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="8" style="30" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="4"/>
+    <col min="5" max="5" width="34" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" style="44" customWidth="1"/>
+    <col min="9" max="10" width="17.140625" style="4"/>
+    <col min="11" max="11" width="30.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="21" customWidth="1"/>
+    <col min="13" max="13" width="56.42578125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" style="21" customWidth="1"/>
     <col min="15" max="15" width="73.42578125" style="4" customWidth="1"/>
     <col min="16" max="16384" width="17.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:25" s="7" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:25" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="19"/>
+      <c r="M3" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54"/>
+      <c r="B4" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="54"/>
+      <c r="B5" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="47" t="s">
+      <c r="I5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="C6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:25" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="C8" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54"/>
+      <c r="C10" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="54"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="19"/>
+      <c r="M11" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="54"/>
+      <c r="B12" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="N2" s="24" t="s">
+      <c r="K12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="54"/>
+      <c r="B13" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="C13" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="N13" s="19"/>
     </row>
-    <row r="3" spans="1:25" s="12" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="36" t="s">
+    <row r="14" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="54"/>
+      <c r="C14" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="54"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="N15" s="19"/>
+    </row>
+    <row r="16" spans="1:25" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="54"/>
+      <c r="C16" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="54"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="1:14" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="54"/>
+      <c r="C18" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="54"/>
+      <c r="B20" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="L20" s="20"/>
+      <c r="M20" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="N20" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="54"/>
+      <c r="B21" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F21" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="54"/>
+      <c r="C22" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M22" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="N22" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="8" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="54"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23" s="19"/>
+      <c r="M23" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="54"/>
+      <c r="B24" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="N24" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="54"/>
+      <c r="B25" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="54"/>
+      <c r="C26" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N26" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="54"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="K27" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L27" s="19"/>
+      <c r="M27" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="54"/>
+      <c r="C28" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="20"/>
+    </row>
+    <row r="29" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="11"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+    </row>
+    <row r="30" spans="1:14" s="8" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="28" t="s">
+      <c r="D30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="56"/>
+      <c r="B31" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="M31" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="N31" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="56"/>
+      <c r="B32" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="I32" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="L32" s="26"/>
+      <c r="M32" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="N32" s="28"/>
+    </row>
+    <row r="33" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="56"/>
+      <c r="B33" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="M33" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="N33" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="56"/>
+      <c r="B34" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="G34" s="16"/>
+      <c r="H34" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="N34" s="26"/>
+    </row>
+    <row r="35" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="56"/>
+      <c r="B35" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="42" t="s">
         <v>188</v>
       </c>
+      <c r="D35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="M35" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>182</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" s="8" t="s">
+    <row r="36" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="56"/>
+      <c r="B36" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E36" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="L36" s="26"/>
+      <c r="M36" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="N36" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="37"/>
+      <c r="B37" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="H38" s="47"/>
+    </row>
+    <row r="39" spans="1:15" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="35"/>
+      <c r="C39" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="N39" s="24"/>
+    </row>
+    <row r="40" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="K40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="27"/>
+      <c r="M40" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="16"/>
+      <c r="K41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="26"/>
+      <c r="M41" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="N41" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="58"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="7"/>
+      <c r="K42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="58"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="52" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="F43" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="I43" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>188</v>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M43" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
-      <c r="B5" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" s="12" t="s">
+    <row r="44" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="58"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E44" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="M44" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N44" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="58"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+    </row>
+    <row r="46" spans="1:15" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:15" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="35"/>
+      <c r="C47" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47" s="24"/>
+      <c r="O47" s="14"/>
+    </row>
+    <row r="48" spans="1:15" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="F48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H48" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="N5" s="28" t="s">
-        <v>188</v>
-      </c>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L48" s="27"/>
+      <c r="M48" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="N48" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="O48" s="7"/>
     </row>
-    <row r="6" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
+    <row r="49" spans="1:15" s="8" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="58"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E49" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="F49" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H49" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="I49" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>9</v>
-      </c>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N49" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="O49" s="16"/>
     </row>
-    <row r="7" spans="1:25" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="13" t="s">
+    <row r="50" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="E50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="I50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L50" s="27"/>
+      <c r="M50" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="N50" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O50" s="7"/>
     </row>
-    <row r="8" spans="1:25" s="8" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
+    <row r="51" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="58"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E51" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="F51" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="H51" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="I51" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="26" t="s">
-        <v>20</v>
-      </c>
+      <c r="J51" s="16"/>
+      <c r="K51" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="L51" s="26"/>
+      <c r="M51" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N51" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O51" s="16"/>
     </row>
-    <row r="9" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="13" t="s">
+    <row r="52" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E52" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="I9" s="12" t="s">
+      <c r="F52" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="I52" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25" t="s">
+      <c r="J52" s="7"/>
+      <c r="K52" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L52" s="27"/>
+      <c r="M52" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="N52" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O52" s="7"/>
     </row>
-    <row r="10" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="9" t="s">
+    <row r="53" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="58"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E53" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="F53" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="16"/>
+      <c r="H53" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="I53" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="26" t="s">
+      <c r="J53" s="16"/>
+      <c r="K53" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="L53" s="26"/>
+      <c r="M53" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="27" t="s">
-        <v>55</v>
-      </c>
+      <c r="N53" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O53" s="16"/>
     </row>
-    <row r="11" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="13" t="s">
+    <row r="54" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="58"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="F54" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="N11" s="28" t="s">
-        <v>99</v>
-      </c>
+      <c r="J54" s="7"/>
+      <c r="K54" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L54" s="27"/>
+      <c r="M54" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N54" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O54" s="7"/>
     </row>
-    <row r="12" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62"/>
-      <c r="B12" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="D12" s="9" t="s">
+    <row r="55" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="58"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E55" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>240</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="N12" s="27"/>
+      <c r="F55" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" s="16"/>
+      <c r="H55" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" s="16"/>
+      <c r="K55" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="L55" s="26"/>
+      <c r="M55" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N55" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O55" s="16"/>
     </row>
-    <row r="13" spans="1:25" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="N13" s="25"/>
-    </row>
-    <row r="14" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" s="12" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="62"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="N15" s="25"/>
-    </row>
-    <row r="16" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="M16" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" s="27"/>
-    </row>
-    <row r="17" spans="1:14" s="12" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="N17" s="25"/>
-    </row>
-    <row r="18" spans="1:14" s="8" customFormat="1" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L18" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="M18" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18" s="27"/>
-    </row>
-    <row r="19" spans="1:14" s="12" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="N19" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="8" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="53" t="s">
-        <v>230</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="N20" s="26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
-      <c r="B21" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="N22" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="12" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="L23" s="25"/>
-      <c r="M23" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N23" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H24" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="N24" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="62"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" s="25"/>
-      <c r="M25" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N25" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="62"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H26" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="L26" s="27"/>
-      <c r="M26" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="N26" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="62"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="K27" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="L27" s="25"/>
-      <c r="M27" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="H28" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" s="27"/>
-      <c r="M28" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="N28" s="26"/>
-    </row>
-    <row r="29" spans="1:14" s="16" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="15"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-    </row>
-    <row r="30" spans="1:14" s="12" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="N30" s="30"/>
-    </row>
-    <row r="31" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="64"/>
-      <c r="B31" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="59" t="s">
-        <v>192</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="M31" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="N31" s="26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="64"/>
-      <c r="B32" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>207</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="56" t="s">
-        <v>211</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="L32" s="32"/>
-      <c r="M32" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="N32" s="34"/>
-    </row>
-    <row r="33" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="64"/>
-      <c r="B33" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="55" t="s">
-        <v>210</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="M33" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="N33" s="26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="64"/>
-      <c r="B34" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="N34" s="32"/>
-    </row>
-    <row r="35" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="64"/>
-      <c r="B35" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="M35" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="N35" s="26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="64"/>
-      <c r="B36" s="50" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>218</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="L36" s="32"/>
-      <c r="M36" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="N36" s="32" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="61"/>
-      <c r="B37" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="N37" s="33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="H38" s="53"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-    </row>
-    <row r="39" spans="1:15" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="18"/>
-      <c r="H39" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="N39" s="30"/>
-    </row>
-    <row r="40" spans="1:15" s="8" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="66"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J40" s="11"/>
-      <c r="K40" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L40" s="33"/>
-      <c r="M40" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="N40" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="66"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="J41" s="20"/>
-      <c r="K41" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L41" s="32"/>
-      <c r="M41" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="N41" s="34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="66"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J42" s="11"/>
-      <c r="K42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N42" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="66"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="M43" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N43" s="34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="66"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="M44" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="N44" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="66"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
-    </row>
-    <row r="46" spans="1:15" s="8" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="37"/>
-      <c r="H46" s="57"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-    </row>
-    <row r="47" spans="1:15" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="49"/>
-      <c r="C47" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="18"/>
-      <c r="H47" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="N47" s="30"/>
-      <c r="O47" s="18"/>
-    </row>
-    <row r="48" spans="1:15" s="8" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="66"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L48" s="33"/>
-      <c r="M48" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="N48" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="O48" s="11"/>
-    </row>
-    <row r="49" spans="1:15" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="66"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G49" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="I49" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="N49" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="O49" s="20"/>
-    </row>
-    <row r="50" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="66"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J50" s="11"/>
-      <c r="K50" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="L50" s="33"/>
-      <c r="M50" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="N50" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="O50" s="11"/>
-    </row>
-    <row r="51" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="66"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J51" s="20"/>
-      <c r="K51" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="L51" s="32"/>
-      <c r="M51" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N51" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="O51" s="20"/>
-    </row>
-    <row r="52" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="66"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J52" s="11"/>
-      <c r="K52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="L52" s="33"/>
-      <c r="M52" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="N52" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="O52" s="11"/>
-    </row>
-    <row r="53" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="66"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="I53" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" s="20"/>
-      <c r="K53" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="L53" s="32"/>
-      <c r="M53" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N53" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="O53" s="20"/>
-    </row>
-    <row r="54" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="66"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G54" s="11"/>
-      <c r="H54" s="55" t="s">
-        <v>145</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J54" s="11"/>
-      <c r="K54" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="L54" s="33"/>
-      <c r="M54" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="N54" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="O54" s="11"/>
-    </row>
-    <row r="55" spans="1:15" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="66"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="G55" s="20"/>
-      <c r="H55" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" s="20"/>
-      <c r="K55" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="L55" s="32"/>
-      <c r="M55" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N55" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="O55" s="20"/>
-    </row>
-    <row r="56" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D125" s="2"/>
-    </row>
-    <row r="126" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D126" s="2"/>
-    </row>
-    <row r="127" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="4:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D132" s="2"/>
-    </row>
+    <row r="56" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:A28"/>
@@ -6279,26 +6012,24 @@
     <hyperlink ref="H31" r:id="rId20"/>
     <hyperlink ref="H11" r:id="rId21"/>
     <hyperlink ref="H23" r:id="rId22"/>
-    <hyperlink ref="H24" r:id="rId23"/>
-    <hyperlink ref="H25" r:id="rId24"/>
-    <hyperlink ref="H26" r:id="rId25"/>
-    <hyperlink ref="H27" r:id="rId26"/>
-    <hyperlink ref="H34" r:id="rId27"/>
-    <hyperlink ref="H35" r:id="rId28"/>
-    <hyperlink ref="H48" r:id="rId29"/>
-    <hyperlink ref="H49" r:id="rId30"/>
-    <hyperlink ref="H50" r:id="rId31"/>
-    <hyperlink ref="H51" r:id="rId32"/>
-    <hyperlink ref="H53" r:id="rId33"/>
-    <hyperlink ref="H54" r:id="rId34"/>
-    <hyperlink ref="H55" r:id="rId35"/>
-    <hyperlink ref="H28" r:id="rId36"/>
-    <hyperlink ref="H7" r:id="rId37"/>
-    <hyperlink ref="H3" r:id="rId38"/>
-    <hyperlink ref="H4" r:id="rId39"/>
-    <hyperlink ref="H37" r:id="rId40"/>
+    <hyperlink ref="H26" r:id="rId23"/>
+    <hyperlink ref="H27" r:id="rId24"/>
+    <hyperlink ref="H34" r:id="rId25"/>
+    <hyperlink ref="H35" r:id="rId26"/>
+    <hyperlink ref="H48" r:id="rId27"/>
+    <hyperlink ref="H49" r:id="rId28"/>
+    <hyperlink ref="H50" r:id="rId29"/>
+    <hyperlink ref="H51" r:id="rId30"/>
+    <hyperlink ref="H53" r:id="rId31"/>
+    <hyperlink ref="H54" r:id="rId32"/>
+    <hyperlink ref="H55" r:id="rId33"/>
+    <hyperlink ref="H28" r:id="rId34"/>
+    <hyperlink ref="H7" r:id="rId35"/>
+    <hyperlink ref="H3" r:id="rId36"/>
+    <hyperlink ref="H4" r:id="rId37"/>
+    <hyperlink ref="H37" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Send message and show restaurant
Write new sendMessageToUser + showRestaurantSuggestion API, update plan
and update document webservice.
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="247">
   <si>
     <t>Header</t>
   </si>
@@ -313,12 +313,6 @@
         }
     }
 }</t>
-  </si>
-  <si>
-    <t>unfollow_a_user</t>
-  </si>
-  <si>
-    <t>Loại 1 người dùng ra khỏi danh sách theo dõi</t>
   </si>
   <si>
     <t>{
@@ -1277,35 +1271,6 @@
     <t>USERS (SETTINGS)</t>
   </si>
   <si>
-    <t>check_user_follow</t>
-  </si>
-  <si>
-    <t>Kiểm tra user hiện tại có đang theo dõi user khác hay không</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "message": {
-            "code": 200,
-            "message": "Success"
-        },
-        "other_normal_type": {
-            "@isFollowing": "1"
-        }
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "message": {
-            "code": 500,
-            "message": "The followee does not already exist or to be disabled."
-        }
-    }
-}</t>
-  </si>
-  <si>
     <t>contact</t>
   </si>
   <si>
@@ -1343,154 +1308,7 @@
     <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/check_friend</t>
   </si>
   <si>
-    <t>send_message</t>
-  </si>
-  <si>
-    <t>Gởi thông điệp (mesage) giữa 2 user trên TasteSync</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/send_message</t>
-  </si>
-  <si>
-    <t>sender_id, recipient_id, message</t>
-  </si>
-  <si>
-    <t>get_list_restaurants_when_wait_for</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/restaurant/get_list_restaurants_when_wait_for</t>
-  </si>
-  <si>
-    <t>check_ask, user_id, page_number</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "list_restaurant_data": [
-            {
-                "other_normal_type": {
-                    "@isDeal": "1",
-                    "@isRestaurantFav": "1",
-                    "@isRestaurantSaved": "1"
-                },
-                "restaurant": {
-                    "@factualRating": "4",
-                    "@priceRange": "300_1000",
-                    "@restaurantCity": "Da nang",
-                    "@restaurantClosetime": "2013-03-20 00:00:00.0",
-                    "@restaurantId": "1",
-                    "@restaurantLat": "24.42342342",
-                    "@restaurantLon": "34.312422343276",
-                    "@restaurantName": "Res 1",
-                    "@restaurantOpentime": "2013-03-20 00:00:00.0",
-                    "@restaurantState": "Da nang",
-                    "@tbdOpentableId": "0"
-                },
-                "user": {
-                    "@about": "This is my demo content for tasteSync app",
-                    "@fbDataApi": "100001192929206",
-                    "@isOnline": "y",
-                    "@maxInvites": "100",
-                    "@tsFirstName": "Tan",
-                    "@tsLastName": "Viet",
-                    "@tsUserEmail": "tanviet@yahoo.com",
-                    "@tsUserId": "1",
-                    "@userCity": "N/A",
-                    "@userCreatedInitialDatetime": "2013-02-18 00:00:00.0",
-                    "@userGender": "m",
-                    "@userId": "1",
-                    "@userPoints": "24",
-                    "@userState": "N/A"
-                },
-                "user_photo": {
-                    "@created": "2013-02-19 00:00:00.0",
-                    "@filename": "1.png",
-                    "@id": "1",
-                    "@userId": "1"
-                }
-            },
-            {
-                "other_normal_type": {
-                    "@isDeal": "1",
-                    "@isRestaurantFav": "1",
-                    "@isRestaurantSaved": "1"
-                },
-                "restaurant": {
-                    "@factualRating": "3",
-                    "@priceRange": "500_2000",
-                    "@restaurantCity": "HCM City",
-                    "@restaurantClosetime": "2013-03-20 00:00:00.0",
-                    "@restaurantId": "2",
-                    "@restaurantLat": "87.12312",
-                    "@restaurantLon": "321.4324234",
-                    "@restaurantName": "Res 2",
-                    "@restaurantOpentime": "2013-03-20 00:00:00.0",
-                    "@restaurantState": "HCM City",
-                    "@tbdOpentableId": "0"
-                }
-            },
-            {
-                "other_normal_type": {
-                    "@isDeal": "0",
-                    "@isRestaurantFav": "1",
-                    "@isRestaurantSaved": "0"
-                },
-                "restaurant": {
-                    "@factualRating": "5",
-                    "@priceRange": "54654",
-                    "@restaurantCity": "Da nang",
-                    "@restaurantClosetime": "2013-04-01 00:00:00.0",
-                    "@restaurantId": "3",
-                    "@restaurantLat": "87.56465",
-                    "@restaurantLon": "43.234324",
-                    "@restaurantName": "Res 3",
-                    "@restaurantOpentime": "2013-04-01 00:00:00.0",
-                    "@restaurantState": "Da nang",
-                    "@tbdOpentableId": "0"
-                },
-                "user": {
-                    "@about": "This is my demo content",
-                    "@fbDataApi": "507096692",
-                    "@isOnline": "y",
-                    "@maxInvites": "100",
-                    "@tsFirstName": "Carick",
-                    "@tsLastName": "Nguyen",
-                    "@tsUserEmail": "viethoavang@gmail.com",
-                    "@tsUserId": "4",
-                    "@userCity": "N/A",
-                    "@userCreatedInitialDatetime": "2013-02-18 16:58:41.0",
-                    "@userGender": "m",
-                    "@userId": "4",
-                    "@userPoints": "0",
-                    "@userState": "N/A"
-                },
-                "user_photo": {
-                    "@created": "2013-02-19 00:00:00.0",
-                    "@filename": "4.png",
-                    "@id": "2",
-                    "@userId": "4"
-                }
-            }
-        ],
-        "message": {
-            "code": 200,
-            "message": "Success"
-        },
-        "pagination": {
-            "@valueCheck": "false"
-        }
-    }
-}</t>
-  </si>
-  <si>
     <t>get_list_restaurants_by_filter</t>
-  </si>
-  <si>
-    <t>Lấy danh sách nhà hàng dựa vào nội dung mà user đã yêu cầu (ở màn hình Ask). 
-Danh sách nhà hàng này được tìm kiếm cho: 
-+ user chưa đăng nhập 
-+ user đã đăng nhập nhưng chưa bao giờ ask 
-+ user đã đăng nhập và đã ask ít nhất là 1 lần (kết quả tìm được sẽ dựa vào nội dung ask gần đây nhất)</t>
   </si>
   <si>
     <t>Lấy danh sách nhà hàng dựa vào bộ lọc Filter ở màn hình Restaurant kết hợp vói nội dung mà user đã yêu cầu (ở màn hình Ask). 
@@ -1796,39 +1614,6 @@
 + contact_id = 3: Restaurant Data
 + contact_id = 4: Request Blogger</t>
     </r>
-  </si>
-  <si>
-    <t>get_all_cities_states</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lấy danh sách các thành phố, bang </t>
-  </si>
-  <si>
-    <t>http://localhost:8080/TasteSync-0.0.1-SNAPSHOT/services/user/get_all_cities_states</t>
-  </si>
-  <si>
-    <t>{
-    "result": {
-        "list_cities": [
-            {
-    "@city": "Anchorage",
-    "@cityId": "1",
-    "@country": "us",
-    "@state": "AK" 
-   },
-   {
-    "@city": "Elmendorf Afb",
-    "@cityId": "10",
-    "@country": "us",
-    "@state": "AK" 
-   }
-        ],
-  "message": {
-            "code": 200,
-            "message": "Success"
-        }
-    }
-}</t>
   </si>
   <si>
     <t>{
@@ -3061,12 +2846,6 @@
     <t>http://localhost:8080/tsws/services/user/add_user_follow</t>
   </si>
   <si>
-    <t>http://localhost:8080/tsws/services/user/unfollow_a_user</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/tsws/services/user/check_user_follow</t>
-  </si>
-  <si>
     <t>Reference data submit at: http://www.mkyong.com/webservices/jax-rs/jax-rs-formparam-example/</t>
   </si>
   <si>
@@ -3617,6 +3396,119 @@
 {
     "successMsg": "no friend"
 }</t>
+  </si>
+  <si>
+    <t>submitFollowUserStatusChange</t>
+  </si>
+  <si>
+    <t>showFollowStatus</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "Setting succesfully!"
+}</t>
+  </si>
+  <si>
+    <t>followeeUserId, followerUserId, statusFlag</t>
+  </si>
+  <si>
+    <t>followerUserId, followeeUserId</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "1"
+}
+OR
+{
+    "successMsg": "0"
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/submitFollowUserStatusChange</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showFollowStatus</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "Sending succesfully!"
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/sendMessageToUser</t>
+  </si>
+  <si>
+    <t>sendMessageToUser</t>
+  </si>
+  <si>
+    <t>senderID, recipientID, content</t>
+  </si>
+  <si>
+    <t>showRestaurantSuggestion</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showRestaurantSuggestion</t>
+  </si>
+  <si>
+    <t>key, userId</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "restaurantId": "002b38d0-e4b5-012e-6305-003048c87378",
+        "factualId": "002b38d0-e4b5-012e-6305-003048c87378",
+        "restaurantName": "Himha Fusion",
+        "factualRating": "4",
+        "priceRange": "2",
+        "restaurantCityId": "10201",
+        "restaurantHours": "{\"monday\":[[\"11:30\",\"16:00\",\"Lunch\"],[\"17:00\",\"23:00\",\"Dinner\"]],\"tuesday\":[[\"11:30\",\"16:00\",\"Lunch\"],[\"17:00\",\"23:00\",\"Dinner\"]],\"wednesday\":[[\"11:30\",\"16:00\",\"Lunch\"],[\"17:00\",\"23:00\",\"Dinner\"]],\"thursday\":[[\"11:30\",\"16:00\",\"Lunch\"],[\"17:00\",\"23:00\",\"Dinner\"]],\"friday\":[[\"11:30\",\"16:00\",\"Lunch\"],[\"17:00\",\"23:00\",\"Dinner\"]],\"saturday\":[[\"12:00\",\"23:00\",\"Dinner\"]],\"sunday\":[[\"12:00\",\"23:00\",\"Dinner\"]]}",
+        "restaurantLat": "41",
+        "restaurantLon": "-74",
+        "sumVoteCount": "0",
+        "sumVoteValue": "0",
+        "tbdOpenTableId": "0"
+    },
+    {
+        "restaurantId": "005bc36b-d7c2-4cb6-8687-7c0be0f496da",
+        "factualId": "005bc36b-d7c2-4cb6-8687-7c0be0f496da",
+        "restaurantName": "Himlzo",
+        "factualRating": "0",
+        "priceRange": "0",
+        "restaurantCityId": "8642",
+        "restaurantHours": "",
+        "restaurantLat": "38",
+        "restaurantLon": "-122",
+        "sumVoteCount": "0",
+        "sumVoteValue": "0",
+        "tbdOpenTableId": "0"
+    },
+    {
+        "restaurantId": "0065c9b2-d7d6-409b-9fb9-ffef5d6f0ef1",
+        "factualId": "0065c9b2-d7d6-409b-9fb9-ffef5d6f0ef1",
+        "restaurantName": "Himalayan Fugi",
+        "factualRating": "0",
+        "priceRange": "0",
+        "restaurantCityId": "8642",
+        "restaurantHours": "",
+        "restaurantLat": "41",
+        "restaurantLon": "-74",
+        "sumVoteCount": "0",
+        "sumVoteValue": "0",
+        "tbdOpenTableId": "0"
+    }
+]</t>
+  </si>
+  <si>
+    <t>Insert new follower user or delete follower from table</t>
+  </si>
+  <si>
+    <t>Check 2 users is follow</t>
+  </si>
+  <si>
+    <t>Send message from user to orther user</t>
+  </si>
+  <si>
+    <t>Show restaurant with 3 characters</t>
   </si>
 </sst>
 </file>
@@ -3731,7 +3623,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -3763,6 +3655,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3771,7 +3672,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3883,59 +3784,59 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -3947,6 +3848,9 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4251,22 +4155,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1"/>
     <col min="2" max="2" width="8" style="30" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="38" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="4"/>
     <col min="5" max="5" width="34" style="4" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="46.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="43.5703125" style="44" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" style="43" customWidth="1"/>
     <col min="9" max="10" width="17.140625" style="4"/>
     <col min="11" max="11" width="30.28515625" style="4" customWidth="1"/>
     <col min="12" max="12" width="31.85546875" style="21" customWidth="1"/>
@@ -4279,28 +4183,28 @@
     <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:25" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
@@ -4315,13 +4219,13 @@
         <v>3</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -4335,14 +4239,14 @@
       <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="59" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>219</v>
+        <v>150</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>198</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
@@ -4351,35 +4255,35 @@
         <v>5</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>146</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="19"/>
       <c r="M3" s="22" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="N3" s="22" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>220</v>
+        <v>150</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>199</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
@@ -4388,33 +4292,33 @@
         <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="46" t="s">
-        <v>166</v>
+      <c r="H4" s="45" t="s">
+        <v>147</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>44</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="20" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>221</v>
+        <v>150</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>200</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>4</v>
@@ -4423,28 +4327,28 @@
         <v>5</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>174</v>
+        <v>153</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>155</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="22" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="C6" s="39" t="s">
+      <c r="A6" s="58"/>
+      <c r="C6" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -4454,10 +4358,10 @@
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>175</v>
+        <v>154</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>156</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>6</v>
@@ -4466,16 +4370,16 @@
         <v>10</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="34"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -4487,8 +4391,8 @@
       <c r="F7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="45" t="s">
-        <v>176</v>
+      <c r="H7" s="44" t="s">
+        <v>157</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>6</v>
@@ -4501,8 +4405,8 @@
       <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:25" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54"/>
-      <c r="C8" s="39" t="s">
+      <c r="A8" s="58"/>
+      <c r="C8" s="38" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -4514,8 +4418,8 @@
       <c r="F8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="47" t="s">
-        <v>177</v>
+      <c r="H8" s="46" t="s">
+        <v>158</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>6</v>
@@ -4531,9 +4435,9 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="34"/>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -4545,8 +4449,8 @@
       <c r="F9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="45" t="s">
-        <v>178</v>
+      <c r="H9" s="44" t="s">
+        <v>159</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>6</v>
@@ -4563,9 +4467,12 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
-      <c r="C10" s="39" t="s">
-        <v>56</v>
+      <c r="A10" s="58"/>
+      <c r="B10" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>227</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>4</v>
@@ -4573,30 +4480,32 @@
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>54</v>
+      <c r="F10" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>55</v>
+        <v>229</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="54"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="38" t="s">
-        <v>96</v>
+      <c r="A11" s="58"/>
+      <c r="B11" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>228</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>4</v>
@@ -4605,32 +4514,32 @@
         <v>5</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>54</v>
+        <v>244</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="22" t="s">
-        <v>98</v>
+        <v>232</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>231</v>
+        <v>150</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>4</v>
@@ -4639,28 +4548,28 @@
         <v>5</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>234</v>
+        <v>212</v>
+      </c>
+      <c r="H12" s="46" t="s">
+        <v>213</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="54"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>232</v>
+        <v>150</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>211</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>4</v>
@@ -4669,27 +4578,27 @@
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="H13" s="45" t="s">
-        <v>235</v>
+        <v>215</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>214</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="54"/>
-      <c r="C14" s="39" t="s">
-        <v>65</v>
+      <c r="A14" s="58"/>
+      <c r="C14" s="38" t="s">
+        <v>63</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>4</v>
@@ -4698,53 +4607,53 @@
         <v>5</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="47" t="s">
         <v>64</v>
+      </c>
+      <c r="H14" s="46" t="s">
+        <v>62</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>46</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="8" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="54"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="34"/>
-      <c r="C15" s="38" t="s">
-        <v>68</v>
+      <c r="C15" s="37" t="s">
+        <v>66</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="45" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:25" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
-      <c r="C16" s="39" t="s">
-        <v>72</v>
+      <c r="A16" s="58"/>
+      <c r="C16" s="38" t="s">
+        <v>70</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>4</v>
@@ -4753,26 +4662,26 @@
         <v>41</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="47" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="H16" s="46" t="s">
+        <v>72</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>44</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="38" t="s">
-        <v>76</v>
+      <c r="C17" s="37" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>4</v>
@@ -4781,32 +4690,32 @@
         <v>5</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="45" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>76</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N17" s="19"/>
     </row>
     <row r="18" spans="1:14" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="54"/>
-      <c r="C18" s="39" t="s">
-        <v>79</v>
+      <c r="A18" s="58"/>
+      <c r="C18" s="38" t="s">
+        <v>77</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>4</v>
@@ -4815,29 +4724,29 @@
         <v>41</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="46" t="s">
         <v>80</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="47" t="s">
-        <v>82</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>44</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="M18" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="38" t="s">
-        <v>86</v>
+      <c r="C19" s="37" t="s">
+        <v>84</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>4</v>
@@ -4846,13 +4755,13 @@
         <v>5</v>
       </c>
       <c r="F19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="45" t="s">
-        <v>88</v>
+      <c r="H19" s="44" t="s">
+        <v>86</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>6</v>
@@ -4862,19 +4771,19 @@
       </c>
       <c r="L19" s="22"/>
       <c r="M19" s="22" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="54"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>222</v>
+        <v>150</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>201</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>4</v>
@@ -4883,33 +4792,33 @@
         <v>5</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="47" t="s">
-        <v>224</v>
+      <c r="H20" s="46" t="s">
+        <v>203</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="L20" s="20"/>
       <c r="M20" s="20" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="54"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>228</v>
+        <v>190</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>207</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>4</v>
@@ -4918,29 +4827,29 @@
         <v>5</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>229</v>
+        <v>209</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>208</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="L21" s="19"/>
       <c r="M21" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="54"/>
-      <c r="C22" s="39" t="s">
-        <v>91</v>
+      <c r="A22" s="58"/>
+      <c r="C22" s="38" t="s">
+        <v>89</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>4</v>
@@ -4949,29 +4858,29 @@
         <v>5</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>91</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="8" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="38" t="s">
-        <v>100</v>
+      <c r="C23" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>4</v>
@@ -4980,35 +4889,35 @@
         <v>5</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>102</v>
+        <v>131</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>96</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L23" s="19"/>
       <c r="M23" s="22" t="s">
         <v>46</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="54"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>239</v>
+        <v>150</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>218</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>4</v>
@@ -5017,31 +4926,31 @@
         <v>5</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H24" s="47" t="s">
-        <v>243</v>
+        <v>220</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>222</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>240</v>
+        <v>150</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>219</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>4</v>
@@ -5050,29 +4959,29 @@
         <v>5</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>244</v>
+        <v>221</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>223</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="L25" s="19"/>
       <c r="M25" s="22" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="54"/>
-      <c r="C26" s="39" t="s">
-        <v>105</v>
+      <c r="A26" s="58"/>
+      <c r="C26" s="38" t="s">
+        <v>99</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>4</v>
@@ -5081,29 +4990,31 @@
         <v>5</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>108</v>
+        <v>100</v>
+      </c>
+      <c r="H26" s="46" t="s">
+        <v>102</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="38" t="s">
-        <v>109</v>
+      <c r="A27" s="58"/>
+      <c r="B27" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>237</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>4</v>
@@ -5112,924 +5023,893 @@
         <v>5</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H27" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="I27" s="9"/>
-      <c r="K27" s="8" t="s">
-        <v>112</v>
+        <v>245</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>238</v>
       </c>
       <c r="L27" s="19"/>
       <c r="M27" s="22" t="s">
-        <v>46</v>
+        <v>235</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>58</v>
+        <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="54"/>
-      <c r="C28" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="5" t="s">
+    <row r="28" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="11"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="1:14" s="8" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="56"/>
+      <c r="B30" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="M30" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="N30" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="56"/>
+      <c r="B31" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="L31" s="26"/>
+      <c r="M31" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="N31" s="28"/>
+    </row>
+    <row r="32" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="56"/>
+      <c r="B32" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="56"/>
+      <c r="B33" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="N33" s="26"/>
+    </row>
+    <row r="34" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="56"/>
+      <c r="B34" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M34" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="56"/>
+      <c r="B35" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="L35" s="26"/>
+      <c r="M35" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="N35" s="28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="53"/>
+      <c r="B36" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4" t="s">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H28" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M28" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="N28" s="20"/>
-    </row>
-    <row r="29" spans="1:14" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="11"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-    </row>
-    <row r="30" spans="1:14" s="8" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="N30" s="24"/>
-    </row>
-    <row r="31" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="56"/>
-      <c r="B31" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="N31" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="56"/>
-      <c r="B32" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>201</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L32" s="26"/>
-      <c r="M32" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="N32" s="28"/>
-    </row>
-    <row r="33" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="56"/>
-      <c r="B33" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>200</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="51" t="s">
-        <v>204</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="M33" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="N33" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="56"/>
-      <c r="B34" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="52" t="s">
-        <v>190</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="N34" s="26"/>
-    </row>
-    <row r="35" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="56"/>
-      <c r="B35" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="M35" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="N35" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="56"/>
-      <c r="B36" s="36" t="s">
-        <v>211</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="50" t="s">
-        <v>214</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="26"/>
-      <c r="M36" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="N36" s="26" t="s">
-        <v>182</v>
+      <c r="N36" s="27" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="H37" s="46"/>
+    </row>
+    <row r="38" spans="1:15" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="N37" s="27" t="s">
-        <v>182</v>
-      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="N38" s="24"/>
     </row>
-    <row r="38" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="H38" s="47"/>
+    <row r="39" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="58"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="K39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="27"/>
+      <c r="M39" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N39" s="25" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="39" spans="1:15" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="13" t="s">
+    <row r="40" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="N39" s="24"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="26"/>
+      <c r="M40" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="N40" s="28" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="40" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="58"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="6" t="s">
+    <row r="41" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" s="7" t="s">
+      <c r="F41" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J40" s="7"/>
-      <c r="K40" s="6" t="s">
+      <c r="J41" s="7"/>
+      <c r="K41" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L40" s="27"/>
-      <c r="M40" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="N40" s="25" t="s">
+      <c r="L41" s="27"/>
+      <c r="M41" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="N41" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="58"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="15" t="s">
+    <row r="42" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="58"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J41" s="16"/>
-      <c r="K41" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L41" s="26"/>
-      <c r="M41" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="N41" s="28" t="s">
-        <v>29</v>
+      <c r="E42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M42" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N42" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="58"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="6" t="s">
+    <row r="43" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="58"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J42" s="7"/>
-      <c r="K42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="N42" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="58"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="16"/>
+      <c r="F43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" s="7"/>
       <c r="H43" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="I43" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="M43" s="28" t="s">
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="M43" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N43" s="28" t="s">
+      <c r="N43" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="58"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="C44" s="41"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="H44" s="50"/>
+      <c r="I44" s="6"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="M44" s="25" t="s">
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+    </row>
+    <row r="45" spans="1:15" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:15" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="F46" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" s="24"/>
+      <c r="O46" s="14"/>
+    </row>
+    <row r="47" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="58"/>
+      <c r="B47" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="H47" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="M47" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="N47" s="20"/>
+    </row>
+    <row r="48" spans="1:15" s="8" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="N48" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="O48" s="16"/>
+    </row>
+    <row r="49" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="58"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" s="7"/>
+      <c r="K49" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L49" s="27"/>
+      <c r="M49" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="N49" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" s="16"/>
+      <c r="K50" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L50" s="26"/>
+      <c r="M50" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="N44" s="25" t="s">
-        <v>47</v>
-      </c>
+      <c r="N50" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="O50" s="16"/>
     </row>
-    <row r="45" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="58"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
+    <row r="51" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="58"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="7"/>
+      <c r="K51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="27"/>
+      <c r="M51" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N51" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="O51" s="7"/>
     </row>
-    <row r="46" spans="1:15" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:15" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="35"/>
-      <c r="C47" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="I47" s="13" t="s">
+    <row r="52" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="I52" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="N47" s="24"/>
-      <c r="O47" s="14"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L52" s="26"/>
+      <c r="M52" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N52" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="O52" s="16"/>
     </row>
-    <row r="48" spans="1:15" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="58"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="6" t="s">
+    <row r="53" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="58"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="I48" s="6" t="s">
+      <c r="F53" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="I53" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="L48" s="27"/>
-      <c r="M48" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="N48" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="O48" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L53" s="27"/>
+      <c r="M53" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N53" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="O53" s="7"/>
     </row>
-    <row r="49" spans="1:15" s="8" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="58"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D49" s="15" t="s">
+    <row r="54" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="58"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E54" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="I49" s="15" t="s">
+      <c r="F54" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="16"/>
+      <c r="H54" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="I54" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="N49" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="O49" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L54" s="26"/>
+      <c r="M54" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N54" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="O54" s="16"/>
     </row>
-    <row r="50" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="58"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J50" s="7"/>
-      <c r="K50" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L50" s="27"/>
-      <c r="M50" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="N50" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="O50" s="7"/>
-    </row>
-    <row r="51" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="58"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G51" s="16"/>
-      <c r="H51" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J51" s="16"/>
-      <c r="K51" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L51" s="26"/>
-      <c r="M51" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N51" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="O51" s="16"/>
-    </row>
-    <row r="52" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G52" s="7"/>
-      <c r="H52" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J52" s="7"/>
-      <c r="K52" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L52" s="27"/>
-      <c r="M52" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="N52" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="O52" s="7"/>
-    </row>
-    <row r="53" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="58"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" s="16"/>
-      <c r="K53" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L53" s="26"/>
-      <c r="M53" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N53" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="O53" s="16"/>
-    </row>
-    <row r="54" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G54" s="7"/>
-      <c r="H54" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J54" s="7"/>
-      <c r="K54" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L54" s="27"/>
-      <c r="M54" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="N54" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="O54" s="7"/>
-    </row>
-    <row r="55" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="58"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" s="16"/>
-      <c r="K55" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="L55" s="26"/>
-      <c r="M55" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N55" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="O55" s="16"/>
-    </row>
-    <row r="56" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A3:A28"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A46:A54"/>
+    <mergeCell ref="A3:A27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1"/>
     <hyperlink ref="H5" r:id="rId2"/>
     <hyperlink ref="H8" r:id="rId3"/>
-    <hyperlink ref="H39" r:id="rId4"/>
-    <hyperlink ref="H40" r:id="rId5"/>
-    <hyperlink ref="H41" r:id="rId6"/>
-    <hyperlink ref="H42" r:id="rId7"/>
-    <hyperlink ref="H43" r:id="rId8"/>
-    <hyperlink ref="H44" r:id="rId9"/>
+    <hyperlink ref="H38" r:id="rId4"/>
+    <hyperlink ref="H39" r:id="rId5"/>
+    <hyperlink ref="H40" r:id="rId6"/>
+    <hyperlink ref="H41" r:id="rId7"/>
+    <hyperlink ref="H42" r:id="rId8"/>
+    <hyperlink ref="H43" r:id="rId9"/>
     <hyperlink ref="H9" r:id="rId10"/>
-    <hyperlink ref="H10" r:id="rId11"/>
-    <hyperlink ref="H47" r:id="rId12"/>
-    <hyperlink ref="H14" r:id="rId13"/>
-    <hyperlink ref="H15" r:id="rId14"/>
-    <hyperlink ref="H16" r:id="rId15"/>
-    <hyperlink ref="H17" r:id="rId16"/>
-    <hyperlink ref="H18" r:id="rId17"/>
-    <hyperlink ref="H19" r:id="rId18"/>
-    <hyperlink ref="H22" r:id="rId19"/>
-    <hyperlink ref="H31" r:id="rId20"/>
-    <hyperlink ref="H11" r:id="rId21"/>
-    <hyperlink ref="H23" r:id="rId22"/>
-    <hyperlink ref="H26" r:id="rId23"/>
-    <hyperlink ref="H27" r:id="rId24"/>
-    <hyperlink ref="H34" r:id="rId25"/>
-    <hyperlink ref="H35" r:id="rId26"/>
-    <hyperlink ref="H48" r:id="rId27"/>
-    <hyperlink ref="H49" r:id="rId28"/>
-    <hyperlink ref="H50" r:id="rId29"/>
-    <hyperlink ref="H51" r:id="rId30"/>
-    <hyperlink ref="H53" r:id="rId31"/>
-    <hyperlink ref="H54" r:id="rId32"/>
-    <hyperlink ref="H55" r:id="rId33"/>
-    <hyperlink ref="H28" r:id="rId34"/>
-    <hyperlink ref="H7" r:id="rId35"/>
-    <hyperlink ref="H3" r:id="rId36"/>
-    <hyperlink ref="H4" r:id="rId37"/>
-    <hyperlink ref="H37" r:id="rId38"/>
+    <hyperlink ref="H14" r:id="rId11"/>
+    <hyperlink ref="H15" r:id="rId12"/>
+    <hyperlink ref="H16" r:id="rId13"/>
+    <hyperlink ref="H17" r:id="rId14"/>
+    <hyperlink ref="H18" r:id="rId15"/>
+    <hyperlink ref="H19" r:id="rId16"/>
+    <hyperlink ref="H22" r:id="rId17"/>
+    <hyperlink ref="H30" r:id="rId18"/>
+    <hyperlink ref="H23" r:id="rId19"/>
+    <hyperlink ref="H26" r:id="rId20"/>
+    <hyperlink ref="H33" r:id="rId21"/>
+    <hyperlink ref="H34" r:id="rId22"/>
+    <hyperlink ref="H48" r:id="rId23"/>
+    <hyperlink ref="H49" r:id="rId24"/>
+    <hyperlink ref="H50" r:id="rId25"/>
+    <hyperlink ref="H52" r:id="rId26"/>
+    <hyperlink ref="H53" r:id="rId27"/>
+    <hyperlink ref="H54" r:id="rId28"/>
+    <hyperlink ref="H7" r:id="rId29"/>
+    <hyperlink ref="H3" r:id="rId30"/>
+    <hyperlink ref="H4" r:id="rId31"/>
+    <hyperlink ref="H36" r:id="rId32"/>
+    <hyperlink ref="H25" r:id="rId33"/>
+    <hyperlink ref="H46" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Profile, restaurant and friend API webservice
showMyProfileHome+ showProfileRestaurants + inviteFriend+
submitUserReport, update Document webservice file, update plan and
create webservice
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="149">
   <si>
     <t>Header</t>
   </si>
@@ -965,12 +965,194 @@
   <si>
     <t>When user login to app in the first. And click "I'm done" button.</t>
   </si>
+  <si>
+    <t>showMyProfileHome</t>
+  </si>
+  <si>
+    <t>Show Profile Home of User</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/getHomeProfile</t>
+  </si>
+  <si>
+    <t>{
+    "name": "Huu Phan",
+    "photo": "https://www.facebook.com/tanhuu94_dn/pic",
+    "facebookCity": "Anchorage",
+    "facebookUrl": "https://www.facebook.com/tanhuu94_dn",
+    "twitterUrl": "",
+    "blogUrl": "",
+    "aboutMeText": "",
+    "numFollowers": "2",
+    "numFollowees": "1",
+    "numFriendsOnTs": "0",
+    "numPoints": "0",
+    "restaurantList": [
+        {
+            "id": "000b79b3-c24f-47ac-83d4-ac49d921d380",
+            "photo": null,
+            "name": "Restaraunt Latino"
+        },
+        {
+            "id": "000b79b3-c24f-47ac-83d4-ac49d921d380",
+            "photo": null,
+            "name": "Restaraunt Latino"
+        },
+        {
+            "id": "002b38d0-e4b5-012e-6305-003048c87378",
+            "photo": {
+                "restaurantId": "002b38d0-e4b5-012e-6305-003048c87378",
+                "photoId": "4eb73eef7ee5024d7fcc4c7f",
+                "prefix": "https://irs1.4sqi.net/img/general/",
+                "suffix": "/NSPHRG4S5LDR53KEL2YOKAGVWW5WDAZGVCGOJCBG2NYG1HS2.jpg",
+                "width": "720",
+                "height": "406",
+                "ultimateSourceName": "foursquare for Android",
+                "ultimateSourceUrl": "https://foursquare.com/download/#/android",
+                "photoSource": "4SQ"
+            },
+            "name": "Alpha Fusion"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>showProfileRestaurants</t>
+  </si>
+  <si>
+    <t>Show list of restaurants which you added to favorite, recommended, saved or left a tips</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/showProfileRestaurants</t>
+  </si>
+  <si>
+    <t>userId, type, from,
+   to</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> type: 0:all; 1:fav; 2:reco; 3:saved; 4:tips</t>
+    </r>
+  </si>
+  <si>
+    <t>[
+    {
+        "restauarntId": "000b79b3-c24f-47ac-83d4-ac49d921d380",
+        "restaurantName": "Restaraunt Latino",
+        "cuisineTier2Name": "American",
+        "price": "2",
+        "restaurantLat": "33",
+        "restaurantLong": "-97",
+        "restaurantDealFlag": null,
+        "restaurantRating": "0",
+        "userSavedFlag": "1",
+        "userFavFlag": "1",
+        "userRecommendedFlag": "0",
+        "userTipFlag": "0",
+        "restaurantCity": {
+            "cityId": "15572",
+            "country": "us",
+            "state": "TX",
+            "city": "Dallas"
+        }
+    },
+    {
+        "restauarntId": "000b79b3-c24f-47ac-83d4-ac49d921d380",
+        "restaurantName": "Restaraunt Latino",
+        "cuisineTier2Name": "American",
+        "price": "2",
+        "restaurantLat": "33",
+        "restaurantLong": "-97",
+        "restaurantDealFlag": null,
+        "restaurantRating": "0",
+        "userSavedFlag": "1",
+        "userFavFlag": "1",
+        "userRecommendedFlag": "0",
+        "userTipFlag": "0",
+        "restaurantCity": {
+            "cityId": "15572",
+            "country": "us",
+            "state": "TX",
+            "city": "Dallas"
+        }
+    },
+    {
+        "restauarntId": "002b38d0-e4b5-012e-6305-003048c87378",
+        "restaurantName": "Alpha Fusion",
+        "cuisineTier2Name": "American",
+        "price": "2",
+        "restaurantLat": "41",
+        "restaurantLong": "-74",
+        "restaurantDealFlag": null,
+        "restaurantRating": "4",
+        "userSavedFlag": "1",
+        "userFavFlag": "0",
+        "userRecommendedFlag": "0",
+        "userTipFlag": "0",
+        "restaurantCity": {
+            "cityId": "11756",
+            "country": "us",
+            "state": "NY",
+            "city": "New York"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>inviteFriend</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/inviteFriend</t>
+  </si>
+  <si>
+    <t>userId, friendFBId</t>
+  </si>
+  <si>
+    <t>Invite Facebook friend</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "Invite Friend Successfully!"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "Reported Successfully!"
+}</t>
+  </si>
+  <si>
+    <t>submitUserReport</t>
+  </si>
+  <si>
+    <t>Report an user</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/submitUserReport</t>
+  </si>
+  <si>
+    <t>userId, reportedUserId, reason</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1044,9 +1226,22 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="20"/>
-      <color theme="3" tint="-0.499984740745262"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1120,7 +1315,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1202,24 +1397,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1247,29 +1427,38 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1277,17 +1466,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1591,22 +1804,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y45"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1"/>
-    <col min="2" max="2" width="8" style="27" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="8" style="51" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="29" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="4"/>
     <col min="5" max="5" width="34" style="4" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="46.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="43.5703125" style="38" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" style="33" customWidth="1"/>
     <col min="9" max="10" width="17.140625" style="4"/>
     <col min="11" max="11" width="30.28515625" style="4" customWidth="1"/>
     <col min="12" max="12" width="31.85546875" style="19" customWidth="1"/>
@@ -1621,10 +1834,10 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1675,13 +1888,13 @@
       <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="28" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1696,7 +1909,7 @@
       <c r="G3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="34" t="s">
         <v>28</v>
       </c>
       <c r="I3" s="9" t="s">
@@ -1714,11 +1927,11 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1731,7 +1944,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="61" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -1749,11 +1962,11 @@
       </c>
     </row>
     <row r="5" spans="1:25" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="53"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="28" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -1765,7 +1978,7 @@
       <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="34" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -1783,11 +1996,11 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="29" t="s">
         <v>104</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1799,7 +2012,7 @@
       <c r="F6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="35" t="s">
         <v>110</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -1816,11 +2029,11 @@
       </c>
     </row>
     <row r="7" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-      <c r="B7" s="30" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="28" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1832,7 +2045,7 @@
       <c r="F7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="34" t="s">
         <v>111</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -1850,11 +2063,11 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="46"/>
+      <c r="B8" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="29" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1866,7 +2079,7 @@
       <c r="F8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="35" t="s">
         <v>90</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -1880,11 +2093,11 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="30" t="s">
+      <c r="A9" s="46"/>
+      <c r="B9" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="28" t="s">
         <v>88</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1896,7 +2109,7 @@
       <c r="F9" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="34" t="s">
         <v>91</v>
       </c>
       <c r="I9" s="8" t="s">
@@ -1912,11 +2125,11 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="29" t="s">
         <v>127</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1928,13 +2141,13 @@
       <c r="F10" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="35" t="s">
         <v>126</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="44" t="s">
         <v>124</v>
       </c>
       <c r="M10" s="19" t="s">
@@ -1945,13 +2158,13 @@
       </c>
     </row>
     <row r="11" spans="1:25" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="33"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="39"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="20"/>
@@ -1959,11 +2172,11 @@
       <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="29" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1976,7 +2189,7 @@
         <v>79</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="35" t="s">
         <v>80</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -1994,11 +2207,11 @@
       </c>
     </row>
     <row r="13" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="46"/>
+      <c r="B13" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="28" t="s">
         <v>84</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -2010,7 +2223,7 @@
       <c r="F13" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="34" t="s">
         <v>85</v>
       </c>
       <c r="I13" s="9" t="s">
@@ -2028,11 +2241,11 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="46"/>
+      <c r="B14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="29" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -2044,7 +2257,7 @@
       <c r="F14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="35" t="s">
         <v>99</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -2061,11 +2274,11 @@
       </c>
     </row>
     <row r="15" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="46"/>
+      <c r="B15" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="28" t="s">
         <v>96</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -2077,7 +2290,7 @@
       <c r="F15" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="34" t="s">
         <v>100</v>
       </c>
       <c r="I15" s="9" t="s">
@@ -2094,22 +2307,50 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="5"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
-      <c r="B17" s="30" t="s">
+    <row r="16" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="46"/>
+      <c r="B16" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>114</v>
+      <c r="C16" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="46"/>
+      <c r="B17" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>4</v>
@@ -2117,625 +2358,741 @@
       <c r="E17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>113</v>
+      <c r="F17" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>135</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="J17" s="9"/>
       <c r="K17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="46"/>
+      <c r="B18" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="46"/>
+      <c r="B19" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="43"/>
+      <c r="H19" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="46"/>
+      <c r="B20" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="20" t="s">
+      <c r="L20" s="4"/>
+      <c r="M20" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N20" s="19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-    </row>
-    <row r="19" spans="1:15" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+    </row>
+    <row r="22" spans="1:15" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B22" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C22" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="41" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12" t="s">
+      <c r="J22" s="12"/>
+      <c r="K22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21" t="s">
+      <c r="L22" s="21"/>
+      <c r="M22" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N19" s="21"/>
-    </row>
-    <row r="20" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
-      <c r="B20" s="28" t="s">
+      <c r="N22" s="21"/>
+    </row>
+    <row r="23" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C23" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="42" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="22" t="s">
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="M20" s="22" t="s">
+      <c r="M23" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N20" s="18" t="s">
+      <c r="N23" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
-      <c r="B21" s="32" t="s">
+    <row r="24" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C24" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="43" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="13" t="s">
+      <c r="J24" s="14"/>
+      <c r="K24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="25" t="s">
+      <c r="L24" s="23"/>
+      <c r="M24" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="25"/>
-    </row>
-    <row r="22" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
-      <c r="B22" s="28" t="s">
+      <c r="N24" s="25"/>
+    </row>
+    <row r="25" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="49"/>
+      <c r="B25" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C25" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="44" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="22" t="s">
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="M22" s="22" t="s">
+      <c r="M25" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N22" s="18" t="s">
+      <c r="N25" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
-      <c r="B23" s="32" t="s">
+    <row r="26" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="49"/>
+      <c r="B26" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C26" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F26" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="45" t="s">
+      <c r="G26" s="14"/>
+      <c r="H26" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I26" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14" t="s">
+      <c r="J26" s="14"/>
+      <c r="K26" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23" t="s">
+      <c r="L26" s="23"/>
+      <c r="M26" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="23"/>
-    </row>
-    <row r="24" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
-      <c r="B24" s="28" t="s">
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="49"/>
+      <c r="B27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C27" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="42" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="22" t="s">
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="M27" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N27" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
-      <c r="B25" s="32" t="s">
+    <row r="28" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="49"/>
+      <c r="B28" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C28" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="43" t="s">
+      <c r="G28" s="42"/>
+      <c r="H28" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I28" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14" t="s">
+      <c r="J28" s="14"/>
+      <c r="K28" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="23"/>
-      <c r="M25" s="25" t="s">
+      <c r="L28" s="23"/>
+      <c r="M28" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N25" s="25" t="s">
+      <c r="N28" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="47"/>
-      <c r="B26" s="28" t="s">
+    <row r="29" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="40"/>
+      <c r="B29" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C29" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="42" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="22" t="s">
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="N26" s="24" t="s">
+      <c r="N29" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="H27" s="40"/>
-    </row>
-    <row r="28" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="52" t="s">
+    <row r="30" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="H30" s="35"/>
+    </row>
+    <row r="31" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-    </row>
-    <row r="29" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="53"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-    </row>
-    <row r="30" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="53"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-    </row>
-    <row r="31" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="53"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="22"/>
-    </row>
-    <row r="32" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-    </row>
-    <row r="33" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="53"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-    </row>
-    <row r="34" spans="1:15" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="53"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-    </row>
-    <row r="35" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52" t="s">
+      <c r="B31" s="53"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="46"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+    </row>
+    <row r="33" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="46"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+    </row>
+    <row r="34" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="46"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="22"/>
+    </row>
+    <row r="35" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="46"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+    </row>
+    <row r="36" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="46"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+    </row>
+    <row r="37" spans="1:15" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="46"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+    </row>
+    <row r="38" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B39" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C39" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F39" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="H36" s="41" t="s">
+      <c r="H39" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="I36" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K39" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="L36" s="21"/>
-      <c r="M36" s="26" t="s">
+      <c r="L39" s="21"/>
+      <c r="M39" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="N36" s="26"/>
-    </row>
-    <row r="37" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="53"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="5"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-    </row>
-    <row r="38" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="53"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="14"/>
-    </row>
-    <row r="39" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="53"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="7"/>
-    </row>
-    <row r="40" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="53"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="14"/>
-    </row>
-    <row r="41" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="53"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="7"/>
-    </row>
-    <row r="42" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="53"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="14"/>
-    </row>
-    <row r="43" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="53"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="7"/>
-    </row>
-    <row r="44" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="14"/>
-    </row>
-    <row r="45" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="N39" s="26"/>
+    </row>
+    <row r="40" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="46"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="5"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+    </row>
+    <row r="41" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="46"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="14"/>
+    </row>
+    <row r="42" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="46"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="46"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="14"/>
+    </row>
+    <row r="44" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="46"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="46"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="14"/>
+    </row>
+    <row r="46" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="46"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="46"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="14"/>
+    </row>
+    <row r="48" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A36:A44"/>
-    <mergeCell ref="A18:O18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="A39:A47"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A3:A20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
-    <hyperlink ref="H20" r:id="rId2"/>
-    <hyperlink ref="H23" r:id="rId3"/>
-    <hyperlink ref="H24" r:id="rId4"/>
+    <hyperlink ref="H23" r:id="rId2"/>
+    <hyperlink ref="H26" r:id="rId3"/>
+    <hyperlink ref="H27" r:id="rId4"/>
     <hyperlink ref="H3" r:id="rId5"/>
     <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="H26" r:id="rId7"/>
+    <hyperlink ref="H29" r:id="rId7"/>
     <hyperlink ref="H15" r:id="rId8"/>
+    <hyperlink ref="H20" r:id="rId9"/>
+    <hyperlink ref="H16" r:id="rId10"/>
+    <hyperlink ref="H17" r:id="rId11"/>
+    <hyperlink ref="H18" r:id="rId12"/>
+    <hyperlink ref="H19" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User Profile and Setting
Friend Profile View, Submit SignUp Detail View and fix WS API
</commit_message>
<xml_diff>
--- a/ws/WS Design Docs/Document WebServices.xlsx
+++ b/ws/WS Design Docs/Document WebServices.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19440" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
   <si>
     <t>Header</t>
   </si>
@@ -1147,12 +1147,29 @@
   <si>
     <t>userId, reportedUserId, reason</t>
   </si>
+  <si>
+    <t>Get userID from user facebook id</t>
+  </si>
+  <si>
+    <t>getUserId</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/tsws/services/user/getUserId</t>
+  </si>
+  <si>
+    <t>UserFBID</t>
+  </si>
+  <si>
+    <t>{
+    "successMsg": "1-20130711170056-27485"
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1315,7 +1332,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1484,6 +1501,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1502,7 +1522,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1595,7 +1618,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1630,7 +1652,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1806,14 +1827,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1"/>
     <col min="2" max="2" width="8" style="45" customWidth="1"/>
@@ -1832,8 +1853,8 @@
     <col min="16" max="16384" width="17.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:25" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="1:25" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1890,8 +1911,8 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:25" s="8" customFormat="1" ht="40.5" customHeight="1" thickTop="1">
+      <c r="A3" s="62" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="46" t="s">
@@ -1929,8 +1950,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
+    <row r="4" spans="1:25" ht="40.5" customHeight="1">
+      <c r="A4" s="58"/>
       <c r="B4" s="45" t="s">
         <v>32</v>
       </c>
@@ -1964,8 +1985,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57"/>
+    <row r="5" spans="1:25" s="8" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A5" s="58"/>
       <c r="B5" s="46" t="s">
         <v>32</v>
       </c>
@@ -1998,8 +2019,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
+    <row r="6" spans="1:25" ht="39" customHeight="1">
+      <c r="A6" s="58"/>
       <c r="B6" s="45" t="s">
         <v>32</v>
       </c>
@@ -2031,8 +2052,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
+    <row r="7" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A7" s="58"/>
       <c r="B7" s="46" t="s">
         <v>32</v>
       </c>
@@ -2065,8 +2086,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57"/>
+    <row r="8" spans="1:25" ht="39" customHeight="1">
+      <c r="A8" s="58"/>
       <c r="B8" s="45" t="s">
         <v>32</v>
       </c>
@@ -2095,8 +2116,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A9" s="58"/>
       <c r="B9" s="46" t="s">
         <v>32</v>
       </c>
@@ -2127,8 +2148,8 @@
       </c>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:25" ht="39" customHeight="1">
+      <c r="A10" s="58"/>
       <c r="B10" s="45" t="s">
         <v>32</v>
       </c>
@@ -2144,7 +2165,7 @@
       <c r="F10" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="63" t="s">
         <v>126</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -2160,22 +2181,43 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+    <row r="11" spans="1:25" s="8" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A11" s="58"/>
+      <c r="B11" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="H11" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>152</v>
+      </c>
       <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-    </row>
-    <row r="12" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
+      <c r="M11" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="39.75" customHeight="1">
+      <c r="A12" s="58"/>
       <c r="B12" s="45" t="s">
         <v>32</v>
       </c>
@@ -2209,8 +2251,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A13" s="58"/>
       <c r="B13" s="46" t="s">
         <v>67</v>
       </c>
@@ -2243,8 +2285,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
+    <row r="14" spans="1:25" ht="39" customHeight="1">
+      <c r="A14" s="58"/>
       <c r="B14" s="45" t="s">
         <v>32</v>
       </c>
@@ -2276,8 +2318,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
+    <row r="15" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A15" s="58"/>
       <c r="B15" s="46" t="s">
         <v>32</v>
       </c>
@@ -2310,8 +2352,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="57"/>
+    <row r="16" spans="1:25" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A16" s="58"/>
       <c r="B16" s="45" t="s">
         <v>32</v>
       </c>
@@ -2339,7 +2381,7 @@
         <v>45</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="19" t="s">
         <v>132</v>
       </c>
       <c r="N16" s="19" t="s">
@@ -2347,8 +2389,8 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
+    <row r="17" spans="1:15" ht="39" customHeight="1">
+      <c r="A17" s="58"/>
       <c r="B17" s="46" t="s">
         <v>32</v>
       </c>
@@ -2385,8 +2427,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="57"/>
+    <row r="18" spans="1:15" ht="39" customHeight="1">
+      <c r="A18" s="58"/>
       <c r="B18" s="45" t="s">
         <v>32</v>
       </c>
@@ -2419,8 +2461,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57"/>
+    <row r="19" spans="1:15" ht="39" customHeight="1">
+      <c r="A19" s="58"/>
       <c r="B19" s="46" t="s">
         <v>32</v>
       </c>
@@ -2455,8 +2497,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="57"/>
+    <row r="20" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A20" s="58"/>
       <c r="B20" s="51" t="s">
         <v>32</v>
       </c>
@@ -2492,25 +2534,25 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-    </row>
-    <row r="22" spans="1:15" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="59" t="s">
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="39" customHeight="1">
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+    </row>
+    <row r="22" spans="1:15" s="8" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A22" s="60" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="47" t="s">
@@ -2529,7 +2571,7 @@
         <v>51</v>
       </c>
       <c r="G22" s="11"/>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="56" t="s">
         <v>49</v>
       </c>
       <c r="I22" s="11" t="s">
@@ -2545,8 +2587,8 @@
       </c>
       <c r="N22" s="21"/>
     </row>
-    <row r="23" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
+    <row r="23" spans="1:15" ht="39" customHeight="1">
+      <c r="A23" s="61"/>
       <c r="B23" s="48" t="s">
         <v>32</v>
       </c>
@@ -2581,8 +2623,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
+    <row r="24" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A24" s="61"/>
       <c r="B24" s="49" t="s">
         <v>32</v>
       </c>
@@ -2615,8 +2657,8 @@
       </c>
       <c r="N24" s="25"/>
     </row>
-    <row r="25" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
+    <row r="25" spans="1:15" ht="39" customHeight="1">
+      <c r="A25" s="61"/>
       <c r="B25" s="48" t="s">
         <v>32</v>
       </c>
@@ -2651,8 +2693,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+    <row r="26" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A26" s="61"/>
       <c r="B26" s="49" t="s">
         <v>32</v>
       </c>
@@ -2685,8 +2727,8 @@
       </c>
       <c r="N26" s="23"/>
     </row>
-    <row r="27" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
+    <row r="27" spans="1:15" ht="39" customHeight="1">
+      <c r="A27" s="61"/>
       <c r="B27" s="48" t="s">
         <v>32</v>
       </c>
@@ -2721,8 +2763,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
+    <row r="28" spans="1:15" s="8" customFormat="1" ht="39" customHeight="1">
+      <c r="A28" s="61"/>
       <c r="B28" s="49" t="s">
         <v>67</v>
       </c>
@@ -2757,7 +2799,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="39" customHeight="1">
       <c r="A29" s="40"/>
       <c r="B29" s="48" t="s">
         <v>32</v>
@@ -2789,13 +2831,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="39" customHeight="1">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="H30" s="35"/>
     </row>
-    <row r="31" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="56" t="s">
+    <row r="31" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A31" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="47"/>
@@ -2812,8 +2854,8 @@
       <c r="M31" s="21"/>
       <c r="N31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="57"/>
+    <row r="32" spans="1:15" ht="39.75" customHeight="1">
+      <c r="A32" s="58"/>
       <c r="B32" s="48"/>
       <c r="C32" s="31"/>
       <c r="D32" s="6"/>
@@ -2828,8 +2870,8 @@
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
     </row>
-    <row r="33" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="57"/>
+    <row r="33" spans="1:15" s="8" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A33" s="58"/>
       <c r="B33" s="49"/>
       <c r="C33" s="32"/>
       <c r="D33" s="13"/>
@@ -2844,8 +2886,8 @@
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
     </row>
-    <row r="34" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="57"/>
+    <row r="34" spans="1:15" ht="41.25" customHeight="1">
+      <c r="A34" s="58"/>
       <c r="B34" s="48"/>
       <c r="C34" s="31"/>
       <c r="D34" s="6"/>
@@ -2860,8 +2902,8 @@
       <c r="M34" s="24"/>
       <c r="N34" s="22"/>
     </row>
-    <row r="35" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57"/>
+    <row r="35" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A35" s="58"/>
       <c r="B35" s="49"/>
       <c r="C35" s="32"/>
       <c r="D35" s="13"/>
@@ -2876,8 +2918,8 @@
       <c r="M35" s="25"/>
       <c r="N35" s="25"/>
     </row>
-    <row r="36" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="57"/>
+    <row r="36" spans="1:15" ht="28.5" customHeight="1">
+      <c r="A36" s="58"/>
       <c r="B36" s="48"/>
       <c r="C36" s="31"/>
       <c r="D36" s="6"/>
@@ -2892,8 +2934,8 @@
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
     </row>
-    <row r="37" spans="1:15" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="57"/>
+    <row r="37" spans="1:15" s="8" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A37" s="58"/>
       <c r="B37" s="49"/>
       <c r="C37" s="32"/>
       <c r="D37" s="13"/>
@@ -2908,9 +2950,9 @@
       <c r="M37" s="25"/>
       <c r="N37" s="25"/>
     </row>
-    <row r="38" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="56" t="s">
+    <row r="38" spans="1:15" ht="39" customHeight="1"/>
+    <row r="39" spans="1:15" s="12" customFormat="1" ht="39" customHeight="1">
+      <c r="A39" s="57" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="47" t="s">
@@ -2943,8 +2985,8 @@
       </c>
       <c r="N39" s="26"/>
     </row>
-    <row r="40" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="57"/>
+    <row r="40" spans="1:15" ht="39" customHeight="1">
+      <c r="A40" s="58"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="H40" s="35"/>
@@ -2952,8 +2994,8 @@
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
     </row>
-    <row r="41" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="57"/>
+    <row r="41" spans="1:15" s="8" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A41" s="58"/>
       <c r="B41" s="49"/>
       <c r="C41" s="32"/>
       <c r="D41" s="13"/>
@@ -2969,8 +3011,8 @@
       <c r="N41" s="23"/>
       <c r="O41" s="14"/>
     </row>
-    <row r="42" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="57"/>
+    <row r="42" spans="1:15" ht="30" customHeight="1">
+      <c r="A42" s="58"/>
       <c r="B42" s="48"/>
       <c r="C42" s="31"/>
       <c r="D42" s="6"/>
@@ -2986,8 +3028,8 @@
       <c r="N42" s="22"/>
       <c r="O42" s="7"/>
     </row>
-    <row r="43" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="57"/>
+    <row r="43" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A43" s="58"/>
       <c r="B43" s="49"/>
       <c r="C43" s="32"/>
       <c r="D43" s="13"/>
@@ -3003,8 +3045,8 @@
       <c r="N43" s="25"/>
       <c r="O43" s="14"/>
     </row>
-    <row r="44" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="57"/>
+    <row r="44" spans="1:15" ht="29.25" customHeight="1">
+      <c r="A44" s="58"/>
       <c r="B44" s="48"/>
       <c r="C44" s="31"/>
       <c r="D44" s="6"/>
@@ -3020,8 +3062,8 @@
       <c r="N44" s="22"/>
       <c r="O44" s="7"/>
     </row>
-    <row r="45" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="57"/>
+    <row r="45" spans="1:15" s="8" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A45" s="58"/>
       <c r="B45" s="49"/>
       <c r="C45" s="32"/>
       <c r="D45" s="13"/>
@@ -3037,8 +3079,8 @@
       <c r="N45" s="25"/>
       <c r="O45" s="14"/>
     </row>
-    <row r="46" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="57"/>
+    <row r="46" spans="1:15" ht="29.25" customHeight="1">
+      <c r="A46" s="58"/>
       <c r="B46" s="48"/>
       <c r="C46" s="31"/>
       <c r="D46" s="6"/>
@@ -3054,8 +3096,8 @@
       <c r="N46" s="22"/>
       <c r="O46" s="7"/>
     </row>
-    <row r="47" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="57"/>
+    <row r="47" spans="1:15" s="8" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A47" s="58"/>
       <c r="B47" s="49"/>
       <c r="C47" s="32"/>
       <c r="D47" s="13"/>
@@ -3071,7 +3113,7 @@
       <c r="N47" s="25"/>
       <c r="O47" s="14"/>
     </row>
-    <row r="48" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:15" ht="28.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A39:A47"/>
@@ -3095,8 +3137,10 @@
     <hyperlink ref="H18" r:id="rId12"/>
     <hyperlink ref="H19" r:id="rId13"/>
     <hyperlink ref="H22" r:id="rId14"/>
+    <hyperlink ref="H10" r:id="rId15"/>
+    <hyperlink ref="H11" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>